<commit_message>
Add cards for chapters 7-9
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - VU Strafrecht I - 1. Klausur (JKU, Austria).xlsx
+++ b/flashcards/Memcode - VU Strafrecht I - 1. Klausur (JKU, Austria).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="172">
   <si>
     <t>Question</t>
   </si>
@@ -19,6 +19,240 @@
     <t>Answer</t>
   </si>
   <si>
+    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Was sind &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;normative &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Tatbestandselemente?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;sind auslegungsbedürftig&lt;/li&gt;&lt;li&gt;Bedürfen der Ausfüllung anhand einer Werteordnung&lt;/li&gt;&lt;li&gt;manchmal enthält das Gesetz selbst Legaldefinitionen&lt;/li&gt;&lt;li&gt;z.B.: geschlechtliche Handlung, fremd, Bereicherungsvorsatz&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Erfolgsdelikte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Delikte, die den Eintritt einer von der &lt;strong&gt;Tathandlung&lt;/strong&gt;, zumindest gedanklich, &lt;strong&gt;abtrennbaren Wirkung &lt;/strong&gt;(Erfolg) in der &lt;strong&gt;Außenwelt &lt;/strong&gt;voraussetzen.  &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Sonderdelikte?&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Welche 2 Arten werden unterschieden?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Verlangen ein bestimmtes Tatsubjekt.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;eigentliche Sonderdelikte&lt;/strong&gt;: Tatsubjekt ist für die Begründung der Strafbarkeit erforderlich  &lt;/li&gt;&lt;li&gt;&lt;strong&gt;uneigentliche Sonderdelikte&lt;/strong&gt;: Tatsubjekt kann den Strafsatz beeinflussen, wirkt also qualifizierend oder privilegierend.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Beispiel: Missbrauch der Amtsgewalt. &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Allgemeindelikte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Delikte, die von jedermann Begangen werden können.&lt;/p&gt;&lt;p&gt;Die meisten Delikte im StGB sind Allgemeindelikte.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein Mischdelikt?&lt;/p&gt;&lt;p&gt;Welche 2 Arten werden unterschieden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Dasselbe Delikt fasst mehrere Begehungsformen wahlweise zusammen, die mit derselben Strafe bedroht sind.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;alternative Mischdelikte&lt;/strong&gt;: das Gesetz umschreibt den Unwert der Tat alternativ durch Sinn- und Wert&lt;strong&gt;gleiche &lt;/strong&gt;Begehungsformen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;kumulative Mischdelikte&lt;/strong&gt;: das Gesetz &lt;strong&gt;fasst &lt;/strong&gt;unter derselben Bezeichnung Begehungsformen mit &lt;strong&gt;unterschiedlichem &lt;/strong&gt;Sinn- und Wertgehalt &lt;strong&gt;zusammen&lt;/strong&gt;, mit dem Ziel auch solche Begehungsformen derselben Strafdrohung zu unterwerfen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Gefährdungsdelikte?&lt;/p&gt;&lt;p&gt;Welche 3 Arten werden unterschieden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Tatbestand ist die Herbeiführung einer bestimmten Gefahr für das Tatobjekt bzw. Rechtsgut.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;konkrete Gefährdungsdelikte&lt;/strong&gt;: Tatbestand setzt &lt;strong&gt;Herbeiführung &lt;/strong&gt;einer tatsächlichen Gefahr für das Tatobjekt voraus, z.B. § 89&lt;/li&gt;&lt;li&gt;&lt;strong&gt;abstrakte Gefährdungsdelikte&lt;/strong&gt;:&lt;strong&gt; blose gedankliche (=theoretisch/abstrakte) Möglichkeit &lt;/strong&gt;das Tatobjekt bzw. Rechtsgut zu beeinträchtigen. Die Gefährdung wird ex lege unwiderleglich vermutet. z.B.: § 91 (Teilnahme an Schlägerei)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;potentielle Gefährdungsdelikte&lt;/strong&gt;: Gefährdungsdelikte sui generis. Tatbestand ist nur erfüllt, wenn die&lt;strong&gt; typische Eignung&lt;/strong&gt; eines &lt;strong&gt;bestimmten Verhaltens&lt;/strong&gt; zur &lt;strong&gt;Herbeiführung einer konkreten Gefahr&lt;/strong&gt; vom Gericht im &lt;strong&gt;Einzelfall festgestellt&lt;/strong&gt; worden ist, z.B.: § 178f (Verbreitung einer übertragbare Krankheit)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Fahrlässigkeitsdelikte? &lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Das Gesetz bedroht &lt;strong&gt;fahrlässiges&lt;/strong&gt; handeln mit Strafe.&lt;/li&gt;&lt;li&gt;Nach &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/7" rel="noopener noreferrer" target="_blank"&gt;§ 7 Abs. 1&lt;/a&gt; ist fahrlässiges Handeln nur dann strafbar wenn der Gesetzgeber dies für ein bestimmtes Delikt ausdrücklich anordnet&lt;/li&gt;&lt;li class="ql-indent-1"&gt;z.B.: es gibt keine fahrlässige Sachbeschädigung&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Verletzungsdelikte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der Eintritt einer Schädigung gehört zum Tatbestand. &lt;/p&gt;&lt;p&gt;z.B.: Tötung, Willensbeugung bei § 105, Vermögensschädigung bei §§ 144, 146, 153&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Zustandsdelikte?&lt;/p&gt;&lt;p&gt;Wann sind sie rechtlich vollendet?&lt;/p&gt;&lt;p&gt;Wann beginnt die Verjährung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Unrecht der Tat erschöpft sich mit der Herbeiführung des rechtswidrigen Zustands.&lt;/li&gt;&lt;li&gt;Sind ab Eintritt des rechtswidrigen Zustands rechtlich vollendet und die Verjährung beginnt.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Dauerdelikte?&lt;/p&gt;&lt;p&gt;Wann gelten sie als rechtlich vollendet?&lt;/p&gt;&lt;p&gt;Können andere Delikte zu Dauerstraftaten werden?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Das Unrecht der Tat beginnt mit der Vornahme der Handlung und endet erst mit dem Aufhören. z.B. § 99 Freiheitsentziehung&lt;/li&gt;&lt;li&gt;Rechtlich vollendet aber schon ab Vornahme&lt;/li&gt;&lt;li&gt;Durch prolongation der Tathandlung können andere Delikte zu Dauerdelikten werden.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Folgen von Dauerdelikten hinsichtlich:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;größe des Unrecht?&lt;/li&gt;&lt;li&gt;Verjährung?&lt;/li&gt;&lt;li&gt;freiwilliger Beendigung?&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Größe des Unrechts steigt mit Dauer der Handlung&lt;/li&gt;&lt;li&gt;Verjährung: Beginnt erst ab Beendigung der Handlung&lt;/li&gt;&lt;li&gt;Freiwillige Beendigung: Täter kann sich nicht auf Rücktritt (§ 16) berufen.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind mehraktige Delikte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Delikte welche sich aus mehreren Tathandlungen zusammensetzen, z.B.: Einbruchsdiebstahl, Raub&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wo geschieht die Abwandlung der Delikte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;idR durch qualifizierende/priviligierende Tatbestandsmerkmale &lt;/li&gt;&lt;li&gt;Manchmal auch erst auf der Stufe der Schuld vorgenommen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein privilegiertes Delikt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Delikte, bei denen das Gesetz an die Abwandlung des Grunddelikts eine mildere Strafe oder sonstige Vergünstigung knüpft.&lt;/li&gt;&lt;li&gt;Das Grunddelikt ist bei Privilegierungen mitanzuführen.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein qualifiziertes Delikt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Delikte, bei denen das Gesetz an die Abwandlung des Grunddelikts eine höhere Strafe knüpft.&lt;/li&gt;&lt;li&gt;Das Grunddelikt ist bei Qualifikationen mitanzuführen.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein Grunddelikt?&lt;/p&gt;&lt;p&gt;Wovon ist es Teil?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Jede Deliktsfamilie basiert auf einem Grunddelikt&lt;/li&gt;&lt;li&gt;Teil der Abstufung der Strafdrohung&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Vorsatz-Fahrlässigkeits-Kombination?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Das Gesetz verlangt für die &lt;strong&gt;Tathandlung &lt;/strong&gt;Vorsatz, für die &lt;strong&gt;Herbeiführung des Erfolgs&lt;/strong&gt; genügt aber Fahrlässigkeit.&lt;/p&gt;&lt;p&gt;z.B.: §§ 83/2, 92/2 sowie erfolgsqualifizierte Delikte&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind erfolgsqualifizierte Delikte?&lt;/p&gt;&lt;p&gt;Welches Prinzip (Rechtsgrundlage) gilt bezüglich der Strafbarkeit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Untergruppe der Erfolgsdelikte&lt;/li&gt;&lt;li&gt;Gesetz sieht eine höhere Strafe vor, wenn &lt;strong&gt;durch die Verwirklichung&lt;/strong&gt; des Grunddelikts (z.B.: Raub, Brandstiftung) &lt;strong&gt;zusätzlich &lt;/strong&gt;eine &lt;strong&gt;besondere Folge der Tat &lt;/strong&gt;herbeigeführt worden ist (= Erfolgsqualifikation)&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/7" rel="noopener noreferrer" target="_blank"&gt;§ 7 Abs 2 StGB&lt;/a&gt;: Bestraft kann nur werden, wer die Folge zumindest Fahrlässig herbeigeführt hat.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Vorsatzdelikte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Das Gesetz bedroht &lt;strong&gt;vorsätzliches &lt;/strong&gt;Handeln mit Strafe, d.h. es verlangt Vorsatz.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind (schlichte) Tätigkeitsdelikte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Delikte, deren Tatbestand sich in der Vornahme eines bestimmten Tuns erschöpft, Erfolg wird nicht vorausgestetzt&lt;/li&gt;&lt;li&gt;Sie können &lt;strong&gt;nicht&lt;/strong&gt; durch Unterlassen begangen werden.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind echte Unterlassungsdelikte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Delikte, bei denen das Gesetz die Nichtvornahme eines gebotenen Tuns mit Strafe bedroht (z.B. Imstichlassen eines Verletzten § 94, Unterlassung der Hilfeleistung § 95)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Begehungsdelikte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Delikte, bei denen das Gesetz ein bestimmtes Tun mit Strafe bedroht.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist teleologische Reduktion?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Tatbestandsmerkmale sind mehr oder weniger auslegungsbedürftig.&lt;/li&gt;&lt;li&gt;Teleologische Reduktion ist jene &lt;strong&gt;Auslegung&lt;/strong&gt;, welche den Anwendungsbereich eines strafrechtlichen Tatbestands bzw. einzelner Tatbestandsmerkmale &lt;strong&gt;mit Blick auf Sinn und Zweck der gesetzlichen Regelung&lt;/strong&gt; hinter den sprachlichen Wortsinn &lt;strong&gt;zurückführt&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;Der Gesetzeswortlaut wird also eingeschränkt.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind &lt;strong&gt;geschriebene &lt;/strong&gt;und &lt;strong&gt;ungeschriebene &lt;/strong&gt;Tatbestandsmerkmale&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Geschriebene Tatbestandsmerkmale&lt;/strong&gt;: der Großteil der Merkmale ist &lt;strong&gt;ausdrücklich &lt;/strong&gt;im&lt;strong&gt; Gesetz festgelegt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Bei einer Reihe von Delikten kommen aber auch &lt;strong&gt;ungeschriebene Tatbestandsmerkmale&lt;/strong&gt; vor.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind &lt;strong&gt;deskriptive &lt;/strong&gt;Tatbestandselemente?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Sinngehalt ist verständlich&lt;/li&gt;&lt;li&gt;bedürfen keiner Erklärung oder Auslegung&lt;/li&gt;&lt;li&gt;z.B.: Mutter, Bruder, beweglich, töten&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der erweiterte Vorsatz?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Über den Tatbildvorsatz hinaus auf bestimmte Ziele gerichtet, die der Täter mit der Begehung der strafbaren Handlung verfolgt (z.B.: Bereicherungsvorsatz)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was muss der Tatbildvorsatz umfassen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Alle Merkmale des objektiven Tatbestands.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der subjektive Tatbestand?&lt;/p&gt;&lt;p&gt;Worauf bezieht er sich?&lt;/p&gt;&lt;p&gt;Was umfasst er?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Innere Tatseite&lt;/li&gt;&lt;li&gt;bezieht sich auf Umstände die im seelischen Bereich des Täters liegen.&lt;/li&gt;&lt;li&gt;umfasst beim Vorsatzdelikt den &lt;strong&gt;Tatbildvorsatz &lt;/strong&gt;und falls verlangt den &lt;strong&gt;erweiterten Vorsatz.&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der objektive Tatbestand?&lt;/p&gt;&lt;p&gt;Wie wird er noch bezeichnet?&lt;/p&gt;&lt;p&gt;Was umfasst er?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Die &lt;strong&gt;äußere &lt;/strong&gt;Tatseite&lt;/li&gt;&lt;li&gt;auch &lt;strong&gt;Tatbild &lt;/strong&gt;genannt&lt;/li&gt;&lt;li&gt;Umfasst das&lt;strong&gt; äußere Erscheinen&lt;/strong&gt; des &lt;strong&gt;deliktischen Geschehens&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Tathandlung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Tatobjekt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erfolg&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Person des Täters&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist Unterlassen im strafrechtlichen Sinn?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Die &lt;strong&gt;Nichtvornahme&lt;/strong&gt; eines &lt;strong&gt;gebotenen &lt;/strong&gt;Tuns.&lt;/li&gt;&lt;li&gt;z.B.: Eltern lassen Ihr Kind verhungern erfülllt den strafrechtlichen Handlungsbegriff.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Tun und Unterlassen?&lt;/p&gt;&lt;p&gt;Erfüllen Sie den strafrechtlichen Handlungsbegriff?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;die beiden Erscheinungsformen der Handlung&lt;/li&gt;&lt;li&gt;Beide erfüllen den Handlungsbegriff&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist vis compulsiva?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;willensbeugende &lt;/strong&gt;Gewalt&lt;/li&gt;&lt;li&gt;Der Zwang ist nicht stark genug um den Willen des Gezwungenen auszuschließen, aber intensiv genug um den Willen zu beugen.&lt;/li&gt;&lt;li&gt;Z.B.: Jemand wird solange bedroht/verprügelt/eingesperrt, bis er die verlangte strafbare Handlung begeht.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist vis absoluta?&lt;/p&gt;&lt;p&gt;Erfüllt sie den strafrechtlichen Handlungsbegriff?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;willensausschließende&lt;/strong&gt;, in diesem Sinn &lt;strong&gt;unwiderstehliche &lt;/strong&gt;Gewalt. &lt;/li&gt;&lt;li&gt;Der Gezwungene ist&lt;strong&gt; physisch nicht in der Lage Widerstand zu leisten,&lt;/strong&gt; daher wird der &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;strafrechtliche Handlungsbegriff nicht erfüllt.&lt;/span&gt;&lt;/li&gt;&lt;li&gt;z.B: jemand wird vor ein Auto gestoßen, die Hand wird zum Testieren gewaltsam geführt.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie werden Körperreflexe für die Ausschlussfunktion abgegrenzt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Fehlreaktionen eines Kraftfahrers &lt;/strong&gt;der von plötzlicher Gefahr überrascht wird, sind in den meisten Fällen vom Willen beherrschbar und erfüllen daher den strafrechtlichen Handlungsbegriff (auch Fehlreaktionen innerhalb der sog. Reaktionszeit)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Automatisierte Handlungen&lt;/strong&gt; sind eintrainierte Verhaltensweisen, bei denen der Wille nicht jedes mal aktiv eingeschalten wird, die Willensaktivierung kann aber jederzeit erfolgen. Deshalb erfüllen Sie den strafrechtlichen Handlungsbegriff. Z.B.: Schalten, Bremsen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Impulsive Handlungen&lt;/strong&gt; kommen zwar unter Umgehung der Tathemmungsmechanismen, nicht aber unter Ausschaltung des Willens zu stande, und erfüllen daher den &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;strafrechtlichen Handlungsbegriff. Z.B.: Affekt- und Kurzschlussreaktionen&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Ausschlussfunktion des strafrechtlichen Handlungsbegriffs?&lt;/p&gt;&lt;p&gt;Was gilt es, besonders bei &lt;strong&gt;kurzzeitigem &lt;/strong&gt;Bewusstseinsverlust, zu beachten?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Für &lt;strong&gt;Schlafende &lt;/strong&gt;und &lt;strong&gt;Bewusstlose&lt;/strong&gt;, bei &lt;strong&gt;Körperreflexen &lt;/strong&gt;und bei &lt;strong&gt;vis absoluta&lt;/strong&gt; fehlt die Möglichkeit der willensmäßigen Beherrschung -&amp;gt; keine Bestrafung.&lt;/li&gt;&lt;li&gt;Es darf bei Schlafenden und Bewusstlosen nicht übersehen werden, dass sie möglicherweise &lt;strong&gt;bereits früher strafbar gehandelt&lt;/strong&gt; haben: z.B: Verkehrsunfall durch Sekundenschlaf -&amp;gt; erfüllt Handlungsbegriff, weil trotz Müdigkeit weitergefahren wurde.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der strafrechtliche Handlungsbegriff?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Eine Handlung iSd strafrechtlichen Handlungsbegriffs ist ein &lt;strong&gt;vom Willen beherrschbares&lt;/strong&gt; menschliches &lt;strong&gt;Verhalten&lt;/strong&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Aufgabe des Strafrechts?&lt;/p&gt;&lt;p&gt;Was steht an der Spitze?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Schutz von Rechtsgütern&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/75" rel="noopener noreferrer" target="_blank"&gt;§ 75 StGB&lt;/a&gt; (Mord) steht an der Spitze&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der &lt;strong style="color: rgb(226, 148, 20); background-color: rgba(0, 0, 0, 0);"&gt;Gesinnungsunwert&lt;/strong&gt;?&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88);"&gt;Welche weiteren Eigenschaften gehören zum &lt;/span&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(226, 148, 20);"&gt;Gesinnungsunwert&lt;/span&gt;&lt;span style="background-color: rgb(40, 45, 88);"&gt;?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Der in der Tat zum Ausdruck kommende &lt;strong&gt;Schuldgehalt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Insbesondere die &lt;strong&gt;Art&lt;/strong&gt; und &lt;strong&gt;Maß &lt;/strong&gt;der durch die Tat dokumentierten &lt;strong&gt;rechtsfeindlichen Einstellung &lt;/strong&gt;und &lt;strong&gt;kriminellen Energie &lt;/strong&gt;(vorsätzliche Tötung [Mord] vs fahrlässige Tötung)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der &lt;strong&gt;Handlungsunwert&lt;/strong&gt;?&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Welche weiteren Eigenschaften gehören zum Handlungsunwert?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Wird durch die &lt;strong&gt;Art &lt;/strong&gt;und &lt;strong&gt;Weise &lt;/strong&gt;der &lt;strong&gt;Tatbegehung &lt;/strong&gt;bestimmt (Wie wurde die Tat begangen)&lt;/li&gt;&lt;li&gt;Dazu gehören auch personale Komponenten (Wer hat die Tat begangen)&lt;/li&gt;&lt;li&gt;Steigt mit Intensität bzw. Brutalität der angewendeten Gewalt, sowie Schwere der eingesetzten Drohung&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Was ist das Fallprüfungsschema?&lt;/p&gt;</t>
   </si>
   <si>
@@ -31,7 +265,7 @@
     <t>&lt;ul&gt;&lt;li&gt;Sämtliche Merkmale des RFG müssen erfüllt sein.&lt;/li&gt;&lt;li&gt;Die Handlung bleibt unrecht/strafbar, wenn die Grenzen des RFg überschritten werden. &lt;/li&gt;&lt;li&gt;RFG wirkt nur &lt;strong&gt;ad personam&lt;/strong&gt; (persönlich), d.h. bei mehreren Beteiligten einer Tat ist nur derjenige gerechtfertigt, der in seiner Person alle Merkmale des RFG erfüllt.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Wie wirken die Rechtfertigungsgründe?&lt;/p&gt;</t>
+    <t>&lt;p&gt;Wie wirken die Rechtfertigungsgründe?&lt;/p&gt;&lt;p&gt;Was ist die Folge?&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;ul&gt;&lt;li&gt;Sie beseitigen nicht die &lt;strong&gt;Tatbestandsmäßigkeit&lt;/strong&gt;, sondern nur das &lt;strong&gt;Unrecht&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;Die Handlung wird von der Rechtsordnung gebilligt, es darf keine Strafe oder vorbeugende Maßnahme verhängt werden. &lt;/li&gt;&lt;/ul&gt;</t>
@@ -64,7 +298,7 @@
     <t>&lt;p&gt;Was sind Rechtfertigungsgründe?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Beschreiben Voraussetzungen, unter denen tatbestandsmäßige Handlungen von der Rechtsordnung gebilligt werden.&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;strong&gt;Voraussetzungen&lt;/strong&gt;, unter denen &lt;strong&gt;tatbestandsmäßige Handlungen &lt;/strong&gt;von der Rechtsordnung &lt;strong&gt;gebilligt &lt;/strong&gt;werden.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was ist der Tatbestand?&lt;/p&gt;&lt;p&gt;Wie wird er noch genannt?&lt;/p&gt;</t>
@@ -79,18 +313,6 @@
     <t>&lt;p&gt;Für die Strafzumessung und Diversion&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist der &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(226, 148, 20);"&gt;Gesinnungsunwert&lt;/strong&gt;?&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88);"&gt;Welche weiteren Eigenschaften gehören zum Handlungsunwert?&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Der in der Tat zum Ausdruck kommende Schuldgehalt&lt;/li&gt;&lt;li&gt;Insbesondere die &lt;strong&gt;Art&lt;/strong&gt; und &lt;strong&gt;Maß &lt;/strong&gt;der durch die Tat dokumentierten &lt;strong&gt;rechtsfeindlichen Einstellung &lt;/strong&gt;und &lt;strong&gt;kriminellen Energie &lt;/strong&gt;(vorsätzliche Tötung [Mord] vs fahrlässige Tötung)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der &lt;strong&gt;Handlungsunwert&lt;/strong&gt;?&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Welche weiteren Eigenschaften gehören zum Handlungsunwert?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Wird durch die Art und Weise der Tatbegehung bestimmt (Wie wurde die Tat begangen)&lt;/li&gt;&lt;li&gt;Dazu gehören auch Personale Komponenten (Wer hat die Tat begangen)&lt;/li&gt;&lt;li&gt;Steigt mit Intensität bzw. Brutalität der angewendeten Gewalt, sowie SChwere der Eingesetzten Drohung&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was ist der &lt;strong&gt;Erfolgsunwert&lt;/strong&gt;?&lt;/p&gt;&lt;p&gt;Welche weiteren &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Eigenschaften &lt;/span&gt;gehören zum Erfolgsunwert?&lt;/p&gt;</t>
   </si>
   <si>
@@ -103,10 +325,10 @@
     <t>&lt;ul&gt;&lt;li&gt;Eine Handlung, die gegen die Rechtsordnung als Ganzes verstößt &lt;/li&gt;&lt;li&gt;Strafhandlung kein unrecht wenn Rechtsordnung sie billigt. Verstöße wie Notwehr, Einwilligung, Anhalterecht, ... &lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist die &lt;span style="color: rgb(226, 148, 20); background-color: rgb(40, 45, 88);"&gt;richterrechtliche&lt;/span&gt; Rechtsfortbildung &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Anwendung der Rechtswissenschaften die über Gesetzesauslegung hinausgeht&lt;/li&gt;&lt;li&gt;Der Reichter schafft dadurch geltendes Recht&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;p&gt;Was ist die &lt;span style="background-color: rgb(40, 45, 88); color: rgb(226, 148, 20);"&gt;richterrechtliche&lt;/span&gt; Rechtsfortbildung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Anwendung der Rechtswissenschaften die über Gesetzesauslegung hinausgeht&lt;/li&gt;&lt;li&gt;Der Richter schafft dadurch geltendes Recht&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was ist das &lt;strong&gt;Verbot strafbegründenden oder strafverschärfenden Gewohnheitsrechts&lt;/strong&gt;?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
@@ -151,12 +373,6 @@
     <t>&lt;ul&gt;&lt;li&gt;objektive Tatseite: äußere böse Handlung&lt;/li&gt;&lt;li&gt;subjektive Tatseite: innerliches Vorhaben (&lt;strong&gt;Vorsatz&lt;/strong&gt;)&lt;/li&gt;&lt;li&gt;Delikt benötigt sowohl objektive als auch subjektive Tatseite.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist die Aufgabe des Strafrechts? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Schutz von Rechtsgütern&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/75" rel="noopener noreferrer" target="_blank"&gt;§ 75 StGB&lt;/a&gt; (Mord) steht an der Spitze&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wer verhängt Kriminalstrafen? &lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
@@ -184,7 +400,7 @@
     <t>&lt;p&gt;Was sind Rechtsgüter?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;sind strafrechtlich geschützte Werte, Einrichtungen und Zustände, die für das ge-ordnete menschliche Zusammenleben unentbehrlich sind.&lt;/p&gt;</t>
+    <t>&lt;p&gt;sind strafrechtlich geschützte Werte, Einrichtungen und Zustände, die für das geordnete menschliche Zusammenleben unentbehrlich sind.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Wie werden Delikte eingeteilt?&lt;/p&gt;&lt;p&gt;Welche 2 Arten gibt es?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
@@ -292,7 +508,7 @@
     <t>&lt;p&gt;Was sind die 4 Schritte des Subsumtionsvorgangs?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;ol&gt;&lt;li&gt;Aufwerfung der Fragestellung&lt;/li&gt;&lt;li&gt;Obersatz&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Definition eines Tatbestands(merkmal)s&lt;/li&gt;&lt;li&gt;Untersatz&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Feststellung ob ein Sachverhalt(selement) dem Tatbestand entspricht&lt;/li&gt;&lt;li&gt;Ergebnis&lt;/li&gt;&lt;/ol&gt;</t>
+    <t>&lt;ol&gt;&lt;li&gt;Aufwerfung der Fragestellung&lt;/li&gt;&lt;li&gt;Obersatz&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Definition eines Tatbestands(merkmal)s&lt;/li&gt;&lt;li&gt;Untersatz&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Feststellung ob ein Sachverhalt(selement) dem Tatbestand entspricht&lt;/li&gt;&lt;li&gt;Schlusssatz = Ergebnis&lt;/li&gt;&lt;/ol&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Materielles vs Formelles Strafrecht&lt;/p&gt;</t>
@@ -700,7 +916,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B86"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -1106,6 +1322,294 @@
         <v>99</v>
       </c>
     </row>
+    <row r="51" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Add cards for chapter 10
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - VU Strafrecht I - 1. Klausur (JKU, Austria).xlsx
+++ b/flashcards/Memcode - VU Strafrecht I - 1. Klausur (JKU, Austria).xlsx
@@ -11,12 +11,96 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
   <si>
     <t>Question</t>
   </si>
   <si>
     <t>Answer</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie unterscheiden sich Kausalität und Schuld?&lt;/p&gt;&lt;p&gt;Was ist vorher zu prüfen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Kausalität&lt;/strong&gt;: es geht darum, ob eine bestimmte Handlung einen bestimmten Erfolg verursacht hat.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Hat weder Wertung noch Vorwurf&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Schuld&lt;/strong&gt;: es geht darum, ob dem Täter der verursachte Erfolg auch rechtlich vorgeworfen werden kann.&lt;/li&gt;&lt;li&gt;Kausalität ist vor Schuld zu prüfen. Mit Verneinung der Kausalität erübrigt sich die Schuldfrage.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die objektive Zurechenbarkeit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der Erfolg ist in spezifisch normativer Weise mit der Handlung verknüpft&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist überholende Kausalität?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ein &lt;strong&gt;später &lt;/strong&gt;vorgenommenes Tun holt das frühere ein und führt &lt;strong&gt;unabhängig &lt;/strong&gt;von jenem den &lt;strong&gt;Erfolg &lt;/strong&gt;herbei. Das &lt;strong&gt;frühere &lt;/strong&gt;Tun wird damit &lt;strong&gt;nicht&lt;/strong&gt; für den &lt;strong&gt;Erfolg &lt;/strong&gt;wirksam und ist nicht &lt;strong&gt;kausal&lt;/strong&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist kumulative Kausalität?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der Erfolg tritt durch das &lt;strong&gt;Zusammenwirken &lt;/strong&gt;mehrerer Handlungen ein. Damit ist jede dieser Handlungen kausal.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist alternative Kausalität?&lt;/p&gt;&lt;p&gt;Was ist die Folge?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Eine Sonderform der realen/nachweislichen Mitkausalität&lt;/li&gt;&lt;li&gt;Der Erfolg wurde durch Handlungen zweier Täter gemeinsam und gleichzeitig herbeigeführt. &lt;/li&gt;&lt;li&gt;Die Gleichzeitigkeit des Erfolgseintrittes ist idR problematisch bzw. nicht nachweisbar&lt;/li&gt;&lt;li&gt;Beide Täter sind nach dem Grundsatz &lt;strong&gt;in dubio pro reo&lt;/strong&gt; nur wegen des versuchten Delikts zu bestrafen (nicht wegen Erfolg)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Gleichwertigkeit der Ursachen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Alle Ursachen sind gleich (äquivalent).&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;D.h.: Jeder Umstand, der auch nur das Geringste dazu beigetragen hat, dass der Erfolg in seiner konkreten Gestalt eingetreten ist, war für diesen Erfolg kausal, also ursächlich&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist Mitkausalität?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Kausalität&lt;/strong&gt; (Ursächlichkeit) wird &lt;strong&gt;nicht &lt;/strong&gt;dadurch&lt;strong&gt; beseitigt&lt;/strong&gt;, dass der Erfolg erst im &lt;strong&gt;Zusammenwirken &lt;/strong&gt;mit &lt;strong&gt;anderen&lt;/strong&gt; &lt;strong&gt;Umständen &lt;/strong&gt;eingetreten ist. Bloße Mitkausalität genügt.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der tatsächliche Kausalverlauf?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der &lt;strong&gt;wirkliche &lt;/strong&gt;Geschehensablauf und Erfolg in seiner &lt;strong&gt;konkreten &lt;/strong&gt;Gestalt. Hypothetische Verläufe bleiben außer Betracht.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Äquivalenztheorie?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ein Tun ist &lt;strong&gt;kausal &lt;/strong&gt;für einen &lt;strong&gt;Erfolg&lt;/strong&gt;, wenn es &lt;strong&gt;nicht weggedacht &lt;/strong&gt;werden kann, ohne dass der &lt;strong&gt;Erfolg &lt;/strong&gt;in seiner konkreten Gestalt &lt;strong&gt;entfällt&lt;/strong&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Kausalität?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wenn ein bestimmtes Verhalten einen bestimmten Erfolg verursacht hat.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was können Tatobjekte sein?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Personen&lt;/li&gt;&lt;li&gt;körperliche und unkörperliche Sachen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der &lt;strong&gt;Erfolg &lt;/strong&gt;einer Tathandlung?&lt;/p&gt;&lt;p&gt;Ist der Erfolg Teil der Handlung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Die zumindest Gedanklich von der Handlung abtrennbare Wirkung in der Außenwelt.&lt;/li&gt;&lt;li&gt;Der Erfolg ist &lt;strong&gt;nicht Teil &lt;/strong&gt;der Tathandlung, die Handlung muss den Erfolg aber &lt;strong&gt;herbeigeführt&lt;/strong&gt; haben.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Kern jeden Tatbestands?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Tathandlung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der objektive Tatbestand?&lt;/p&gt;&lt;p&gt;Was ist ein zentrales Element davon?&lt;/p&gt;&lt;p&gt;Ist dieses üblicherweise geschrieben oder ungeschrieben?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Die &lt;strong&gt;Summe&lt;/strong&gt; aller &lt;strong&gt;objektiven Tatbestandsmerkmale&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;Zentrales Element: &lt;strong&gt;Kausalität&lt;/strong&gt;. Wird im Gesetz nur ausnahmsweise angesprochen, zählt normalerweise zu den &lt;strong&gt;ungeschriebenen &lt;/strong&gt;Merkmalen.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Was sind &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;normative &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Tatbestandselemente?&lt;/span&gt;&lt;/p&gt;</t>
@@ -916,7 +1000,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B86"/>
+  <dimension ref="A1:B100"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -1610,6 +1694,118 @@
         <v>171</v>
       </c>
     </row>
+    <row r="87" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Add cards for chapter 11
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - VU Strafrecht I - 1. Klausur (JKU, Austria).xlsx
+++ b/flashcards/Memcode - VU Strafrecht I - 1. Klausur (JKU, Austria).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="236">
   <si>
     <t>Question</t>
   </si>
@@ -19,6 +19,120 @@
     <t>Answer</t>
   </si>
   <si>
+    <t>&lt;p&gt;Was ist das Problem des &lt;strong&gt;Vorsatzes trotz Schuldunfähigkeit&lt;/strong&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Vorsatz benötigt nur &lt;strong&gt;Willensfähigkeit &lt;/strong&gt;(Fähigkeit einen Willen zu bilden)&lt;/li&gt;&lt;li&gt;Schuldunfähige können daher vorsätzlich handeln.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Welche 2 Verfehlungen des maßgebenden Zeitpunkts gibt es?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(226, 148, 20);"&gt;dolus &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(226, 148, 20);"&gt;subsequens&lt;/strong&gt;: nach Abschluss der Tat gefasster Vorsatz reicht nicht&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(226, 148, 20);"&gt;dolus &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(226, 148, 20);"&gt;antecedens&lt;/strong&gt;: zum Zeitpunkt der Vornahme bereits aufgegebener Vorsatz reicht nicht&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Problem des &lt;strong&gt;maßgebenden Zeitpunkts&lt;/strong&gt;?&lt;/p&gt;&lt;p&gt;Wie verhält sich dies bei &lt;strong&gt;mehraktigen&lt;/strong&gt;,&lt;strong&gt; Dauer&lt;/strong&gt;-&lt;strong&gt; &lt;/strong&gt;und &lt;strong&gt;Erfolgs&lt;/strong&gt;delikten?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Vorsatz muss zur Zeit der Tat, d.h. bei Vornahme der Tathandlung vorliegen.&lt;/li&gt;&lt;li&gt;Bei Deliktarten:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Mehraktige&lt;/strong&gt;: bereits beim ersten Akt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Dauer&lt;/strong&gt;: kann erst später (aber während Andauern) gefasst werden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erfolg&lt;/strong&gt;: bei Vornahme der Tathandlung reicht, bei Erfolgseintritt nicht gefordert.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Problem des &lt;strong&gt;bedingten&lt;/strong&gt; &lt;strong&gt;Handlungswillen&lt;/strong&gt;?&lt;/p&gt;&lt;p&gt;Beispiele?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Tatvorsatz benötigt &lt;strong&gt;un&lt;/strong&gt;bedingten Handlungswillen&lt;/li&gt;&lt;li&gt;Ist der Wille nur bedingt, liegt kein Vorsatz vor.&lt;/li&gt;&lt;li&gt;Beispiele:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;erklärte Gewaltbereitschaft ist noch kein Vorsatz&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Drohen mit Waffe ist kein unbedingter Handlungswille, auch ein versehentlicher Schuss ist dann kein Vorsatz.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was bedeutet Absichtlichkeit?&lt;/p&gt;&lt;p&gt;Was ist die lat. Bezeichnung?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;dolus specialis&lt;/li&gt;&lt;li&gt;Absichtlich handelt, wem es &lt;strong&gt;darauf ankommt&lt;/strong&gt;, dass er einen Sachverhalt verwirklicht, der einem &lt;strong&gt;gesetzlichen Tatbild &lt;/strong&gt;entspricht&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was bedeutet Wissentlichkeit?&lt;/p&gt;&lt;p&gt;Was ist die lat. Bezeichnung?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;dolus principalis&lt;/li&gt;&lt;li&gt;Wissentlich handelt, &lt;strong&gt;nicht es bloß für möglich hält&lt;/strong&gt;, sondern sein &lt;strong&gt;für gewiss hält, &lt;/strong&gt;dass er einen Sachverhalt verwirklicht, der einem &lt;strong&gt;gesetzlichen Tatbild&lt;/strong&gt; entspricht&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was bedeutet bedingter Vorsatz?&lt;/p&gt;&lt;p&gt;Was ist die lat. Bezeichnung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;dolus eventualis&lt;/li&gt;&lt;li&gt;Bedingt vorsätzlich handelt, wer es zumindest für &lt;strong&gt;möglich hält&lt;/strong&gt;, dass er einen Sachverhalt verwirklicht, der einem &lt;strong&gt;gesetzlichen&lt;/strong&gt; &lt;strong&gt;Tatbild &lt;/strong&gt;entspricht, und sich damit &lt;strong&gt;abfindet&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die drei Stufen des Vorsatzes?&lt;/p&gt;&lt;p&gt;Welche Stufe genügt idR?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Bedingter Vorsatz: geringster Stärkegrad&lt;/li&gt;&lt;li&gt;Wissentlichkeit: mittlerer Stärkegrad&lt;/li&gt;&lt;li&gt;Absichtlichkeit: höchster Stärkegrad&lt;/li&gt;&lt;li&gt;Es genügt idR bedingter Vorsatz gem &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/7" rel="noopener noreferrer" target="_blank"&gt;§&amp;nbsp;7 (1) &lt;/a&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/7" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;StGB&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; &lt;/span&gt;iVm &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/5" rel="noopener noreferrer" target="_blank"&gt;§&amp;nbsp;5/1 2. HS StGB&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Wollenskomponente?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der Täter muss die &lt;strong&gt;Verwirklichung &lt;/strong&gt;des &lt;strong&gt;Tatbildes wollen&lt;/strong&gt;, und sich zumindest mit der &lt;strong&gt;Verletzung &lt;/strong&gt;des &lt;strong&gt;Rechtsguts abfinden&lt;/strong&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie Verhält sich der Vorsatz um Kausalverlauf?&lt;/p&gt;&lt;p&gt;Wie sieht die hL dies im Detail?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Vorsatz muss sich auch auf den &lt;strong&gt;Kausalverlauf &lt;/strong&gt;(Teil des objektiven Tatbestands) &lt;strong&gt;beziehen&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;hl sagt: Kenntnis des Kausalverlaufs in &lt;strong&gt;wesentlichen Zügen&lt;/strong&gt; &lt;strong&gt;genügt&lt;/strong&gt;, Kenntnis der &lt;strong&gt;Einzelheiten nicht erfordert&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Parallelwertung in der Laiensphäre?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Die Wissenskomponente erfordert keine juristisch korrekte Beurteilung, es genügt, wenn die&lt;strong&gt; laienmäßige Einschätzung des Tatbestandes sowie dessen sozialer und rechtlicher Bedeutung&lt;/strong&gt; jener des Rechts parallel läuft.&lt;/li&gt;&lt;li&gt;Beispiel: Täter muss nicht wissen, dass das Herauslassen von Luft aus Autoreifen bereits Sachbeschädigung ist, es genügt zu wissen, dass es einige Mühe kostet, das Auto wieder fahrbereit zu machen.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Besonderheit der Wissenskomponente in Hinblick auf das Wissen des Täters über das Gesetz? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Der Täter muss die &lt;strong&gt;Wertungen &lt;/strong&gt;des Gesetzes &lt;strong&gt;nachvollziehen&lt;/strong&gt; und in ihrem &lt;strong&gt;sozialen&lt;/strong&gt; &lt;strong&gt;Bedeutungsgehalt erfassen&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;Dazu ist keine juristisch korrekte Beurteilung notwendig, die sogenannte &lt;strong&gt;Parallelwertung in der Laiensphäre &lt;/strong&gt;reicht aus.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie unterteilen Lehre (und Praxis) die Wissenskomponente?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Aktualwissen&lt;/strong&gt;: Der Täter hat an die Verwirklichung des Tatbestands oder eines bestimmten Tatbestandsmerkmals &lt;strong&gt;explizit &lt;/strong&gt;gedacht.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Begleitwissen&lt;/strong&gt; (Mitbewusstsein): Dem Täter war die Verwirklichung des Tatbestands oder eines bestimmten Tatbestands aus den &lt;strong&gt;Begleitumständen oder sonst latent bewusst.&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;z.B.: Brieftaschendieb wirft Personalausweis aus gestohlener Tasche weg. Er denkt nicht daran, dass er eine fremde Urkunde unterdrückt, die Tatsache ist ihm jedoch latent Bewusst und er ist zu strafen. &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was umfasst die Wissenskomponente?&lt;/p&gt;&lt;p&gt;Was ist die Mindestanforderung an Wissen? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Kenntnis aller Tatsachen, auf welche sich der objektive Tatbestand bezieht.&lt;/li&gt;&lt;li&gt;Bereits &lt;strong&gt;undeutliche &lt;/strong&gt;und &lt;strong&gt;unreflektierte Vorstellungen &lt;/strong&gt;genügen den Anforderungen des Wissens&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Aus welchen 2 Komponenten besteht der Vorsatz?&lt;/p&gt;&lt;p&gt;Wie sind diese in der Legaldefinition geregelt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Wissens&lt;/strong&gt;- (kognitives Element) und &lt;strong&gt;Wollens&lt;/strong&gt;komponente (voluntatives Element)&lt;/li&gt;&lt;li&gt;§&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/5" rel="noopener noreferrer" target="_blank"&gt; 5 Abs 1 1. HS&lt;/a&gt; erwähnt nur die Wollenskomponente, die Wissenskomponente ist &lt;strong&gt;denknotwendig &lt;/strong&gt;mitenthalten&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was muss der Vorsatz umfassen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Tathandlung&lt;/li&gt;&lt;li&gt;Tatobjekt&lt;/li&gt;&lt;li&gt;allfällige Tatmodalitäten&lt;/li&gt;&lt;li&gt;Erfolg&lt;/li&gt;&lt;li&gt;Kausalverlauf in groben Zügen&lt;/li&gt;&lt;li&gt;etwaige Deliktsqualifikationen (z.B.: Wertqualifikationen)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Stufen des Vorsatzes gibt es?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;Bedingter Vorsatz&lt;/li&gt;&lt;li&gt;Absicht&lt;/li&gt;&lt;li&gt;Wissentlichkeit&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine vorsätzliche Handlung?&lt;/p&gt;&lt;p&gt;Was ist die gesetzliche Grundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Vorsätzlich handelt, wer einen Sachverhalt verwirklichen will, der einem geseztlichen Tatbild entspricht (&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/5" rel="noopener noreferrer" target="_blank"&gt;§ 5 Abs 1 StGB&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der objektive Tatbestand?&lt;/p&gt;&lt;p&gt;Wie wird er noch bezeichnet?&lt;/p&gt;&lt;p&gt;Was umfasst er?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Die &lt;strong&gt;äußere &lt;/strong&gt;Tatseite, die &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(226, 148, 20);"&gt;Summe&lt;/span&gt; aller &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(226, 148, 20);"&gt;objektiven Tatbestandsmerkmale eines Delikts&lt;/span&gt;&lt;/li&gt;&lt;li&gt;auch &lt;strong&gt;Tatbild &lt;/strong&gt;genannt&lt;/li&gt;&lt;li&gt;Umfasst das&lt;strong&gt; äußere Erscheinen&lt;/strong&gt; des &lt;strong&gt;deliktischen Geschehens&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Tathandlung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Tatobjekt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erfolg&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Person des Täters&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Wie unterscheiden sich Kausalität und Schuld?&lt;/p&gt;&lt;p&gt;Was ist vorher zu prüfen?&lt;/p&gt;</t>
   </si>
   <si>
@@ -97,10 +211,10 @@
     <t>&lt;p&gt;Die Tathandlung&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist der objektive Tatbestand?&lt;/p&gt;&lt;p&gt;Was ist ein zentrales Element davon?&lt;/p&gt;&lt;p&gt;Ist dieses üblicherweise geschrieben oder ungeschrieben?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Die &lt;strong&gt;Summe&lt;/strong&gt; aller &lt;strong&gt;objektiven Tatbestandsmerkmale&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;Zentrales Element: &lt;strong&gt;Kausalität&lt;/strong&gt;. Wird im Gesetz nur ausnahmsweise angesprochen, zählt normalerweise zu den &lt;strong&gt;ungeschriebenen &lt;/strong&gt;Merkmalen.&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;p&gt;Was ist ein zentrales Element des objektiven Tatbestands davon?&lt;/p&gt;&lt;p&gt;Ist dieses üblicherweise geschrieben oder ungeschrieben?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Kausalität&lt;/strong&gt;. Wird im Gesetz nur ausnahmsweise angesprochen, zählt normalerweise zu den &lt;strong&gt;ungeschriebenen &lt;/strong&gt;Merkmalen.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Was sind &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;normative &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Tatbestandselemente?&lt;/span&gt;&lt;/p&gt;</t>
@@ -268,13 +382,7 @@
     <t>&lt;p&gt;Was ist der subjektive Tatbestand?&lt;/p&gt;&lt;p&gt;Worauf bezieht er sich?&lt;/p&gt;&lt;p&gt;Was umfasst er?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;ul&gt;&lt;li&gt;Innere Tatseite&lt;/li&gt;&lt;li&gt;bezieht sich auf Umstände die im seelischen Bereich des Täters liegen.&lt;/li&gt;&lt;li&gt;umfasst beim Vorsatzdelikt den &lt;strong&gt;Tatbildvorsatz &lt;/strong&gt;und falls verlangt den &lt;strong&gt;erweiterten Vorsatz.&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der objektive Tatbestand?&lt;/p&gt;&lt;p&gt;Wie wird er noch bezeichnet?&lt;/p&gt;&lt;p&gt;Was umfasst er?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Die &lt;strong&gt;äußere &lt;/strong&gt;Tatseite&lt;/li&gt;&lt;li&gt;auch &lt;strong&gt;Tatbild &lt;/strong&gt;genannt&lt;/li&gt;&lt;li&gt;Umfasst das&lt;strong&gt; äußere Erscheinen&lt;/strong&gt; des &lt;strong&gt;deliktischen Geschehens&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Tathandlung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Tatobjekt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erfolg&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Person des Täters&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;ul&gt;&lt;li&gt;Innere Tatseite, die  Summer aller subjektiven Tatbestandselemente eines Delikts&lt;/li&gt;&lt;li&gt;bezieht sich auf Umstände die im seelischen Bereich des Täters liegen.&lt;/li&gt;&lt;li&gt;umfasst beim Vorsatzdelikt den &lt;strong&gt;Tatbildvorsatz &lt;/strong&gt;und falls verlangt den &lt;strong&gt;erweiterten Vorsatz.&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist Unterlassen im strafrechtlichen Sinn?&lt;/span&gt;&lt;/p&gt;</t>
@@ -1000,7 +1108,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B100"/>
+  <dimension ref="A1:B118"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -1806,6 +1914,150 @@
         <v>199</v>
       </c>
     </row>
+    <row r="101" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Add cards for chapters 12 and 13
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - VU Strafrecht I - 1. Klausur (JKU, Austria).xlsx
+++ b/flashcards/Memcode - VU Strafrecht I - 1. Klausur (JKU, Austria).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="322">
   <si>
     <t>Question</t>
   </si>
@@ -19,6 +19,282 @@
     <t>Answer</t>
   </si>
   <si>
+    <t>&lt;p&gt;Wie gilt "in dubio pro reo" bei Notwehr? &lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sind &lt;strong&gt;sichere Feststellungen &lt;/strong&gt;zu &lt;strong&gt;notwehrerheblichen Umständen &lt;/strong&gt;nicht möglich, darf dies &lt;strong&gt;nicht zulasten des Verteidigers &lt;/strong&gt;gehen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ist Nothilfe &lt;strong&gt;gegen den erkennbaren Willen&lt;/strong&gt; des Angegriffenen zulässig?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nein&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist Nothilfe?&lt;/p&gt;&lt;p&gt;Was ist die gesetzliche Grundlage?&lt;/p&gt;&lt;p&gt;Wie sind die &lt;strong&gt;Voraussetzungen des Angriffs&lt;/strong&gt; zu Beurteilen und bei wem muss das &lt;strong&gt;subjektive&lt;/strong&gt; &lt;strong&gt;Rechtfertigungselement &lt;/strong&gt;gegeben sein?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Notwehr z&lt;strong&gt;ugunsten eines Dritten&lt;/strong&gt;, wie Notwehr gem &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/3" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 3 StGB&lt;/a&gt; ("von sich oder einem anderen")&lt;/li&gt;&lt;li&gt;Die &lt;strong&gt;Voraussetzungen&lt;/strong&gt; &lt;strong&gt;des Angriffs&lt;/strong&gt; sind nach der Person zu beurteilen,&lt;strong&gt; der geholfen wird.&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Das &lt;strong&gt;subjektive&lt;/strong&gt; &lt;strong&gt;Rechtfertigungselement &lt;/strong&gt;muss beim &lt;strong&gt;Nothelfer &lt;/strong&gt;gegeben sein.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Schränkt &lt;a href="https://www.jusline.at/gesetz/emrk/paragraf/artikel2" rel="noopener noreferrer" target="_blank"&gt;Art 2 Abs 1 EMKR&lt;/a&gt; die Notwehrrechte einzelner Staatsbürger gegenüber &lt;strong&gt;Vermögenstätern &lt;/strong&gt;ein?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nein, dies bezieht sich nur auf hoheitliches Handeln des Staats.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist Bagatellnotwehr?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/3" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 3 (1) S2 StGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;offensichtlich bloß geringer Nachteil für den Angegriffenen und die Verteidigung unangemessen → Keine Notwehr&lt;/li&gt;&lt;li&gt;z.B.: Schuss auf Apfeldieb ist einzige Möglichkeit Angriff auf Eigentum abzuwehren → nicht zulässig! &lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Schließen Zorn, Wut, Hass oder Vorsatz den Angreifer zu misshandeln/verletzen Notwehr aus?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nein, wird dadurch nicht &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/3" rel="noopener noreferrer" target="_blank"&gt;§ 3 StGB&lt;/a&gt; ausgeschlossen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das subjektive Rechtfertigungselement?&lt;/p&gt;&lt;p&gt;Was passiert, wenn es nicht vorliegt, was ist die Rechtsgrundlage? &lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Erfordert zumindest &lt;strong&gt;Wissen um das Vorliegen&lt;/strong&gt; der Notwehrsituation&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erkennt &lt;/strong&gt;der Täter die Notwehrsituation gar &lt;strong&gt;nicht&lt;/strong&gt;, ist er für die &lt;strong&gt;vollendete Tat&lt;/strong&gt;, aber &lt;strong&gt;milder&lt;/strong&gt;, zu bestrafen (&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/34" rel="noopener noreferrer" target="_blank"&gt;§&amp;nbsp;34/1 Z11&lt;/a&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Rechtsgrundlage für den Entschuldigungsgrund für intensiven Notwehrexzess?&lt;/p&gt;&lt;p&gt;Wie wird dann gehaftet?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;§&amp;nbsp;3 (2) StGB&lt;/li&gt;&lt;li&gt;Gehaftet wegen &lt;strong&gt;Fahrlässigkeit&lt;/strong&gt;, falls die &lt;strong&gt;Überschreitung auf Fahrlässigkeit beruht&lt;/strong&gt; und ein &lt;strong&gt;entsprechendes Fahrlässigkeitsdelikt&lt;/strong&gt; &lt;strong&gt;existiert&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Notwehrexzess gilt nur bei &lt;strong&gt;gegebener&lt;/strong&gt; Notwehrlage. Wie nennt man Übermaßreaktionen bei irrtümlicher Annahme einer Notwehrsituation? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Putativnotwehrexzess&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist Notwehrexzess (Überschreitung)?&lt;/p&gt;&lt;p&gt;Welche 2 Arten gibt es?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Aus Notwehrhandlung wird &lt;strong&gt;rechtswidriger Angriff&lt;/strong&gt;, gegen den Notwehr zulässig ist.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;intensiver &lt;/strong&gt;Exzess: Verteidiger &lt;strong&gt;überschreitet das&lt;/strong&gt; &lt;strong&gt;Maß &lt;/strong&gt;des zur Abwehr Notwendigen.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;extensiver&lt;/strong&gt; Exzess: Verteidiger &lt;strong&gt;überschreitet die zeitlichen Grenzen&lt;/strong&gt; (kein gegenwärtiger Angriff mehr)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die &lt;strong&gt;Immanenten Schranken &lt;/strong&gt;der Notwehr?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Strafmündigen&lt;/strong&gt;, &lt;strong&gt;Geisteskranken &lt;/strong&gt;und sonst &lt;strong&gt;offensichtlich schuldlos Handelnden&lt;/strong&gt; (&lt;em&gt;nicht&lt;/em&gt; aber Betrunkene!) muss man ausweichen, wenn man dadurch den Angriff verhindern kann.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Abwehrmindernde Vorhandlungen&lt;/strong&gt;: Wer sich selbst ins Unrecht gesetzt hat, muss Minderungen seiner Notwehrbefugnisse hinnehmen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Nothwehrprovokation&lt;/strong&gt;: Wer den Angriff absichtlich herausfordert, verwirkt idR das Notwehrrecht&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das &lt;strong&gt;Schonungsprinzip&lt;/strong&gt;?&lt;/p&gt;&lt;p&gt;Welche mittel sind ausgenommen? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Der Verteidiger muss &lt;strong&gt;unter&lt;/strong&gt; &lt;strong&gt;mehreren&lt;/strong&gt; &lt;strong&gt;wirksamen &lt;/strong&gt;Mitteln das für den Angreifer am &lt;strong&gt;wenigsten gefährliche &lt;/strong&gt;auswählen.&lt;/li&gt;&lt;li&gt;Ausgenommen sind Mittel, deren &lt;strong&gt;Abwehrwirkung&lt;/strong&gt; &lt;strong&gt;zweifelhaft &lt;/strong&gt;sind.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Abwägungen werden in die Notwendigkeit einbezogen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Gesamt&lt;/strong&gt;abwägung&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Güter&lt;/strong&gt;abwägung nur in&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/3" rel="noopener noreferrer" target="_blank"&gt; §&amp;nbsp;3 (1) S2 StGB&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wonach richtet sich die Notwendigkeit?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Notwendigkeit richtet sich nach der &lt;strong&gt;Gefährlichkeit&lt;/strong&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie wird die Notwendigkeit einer Abwehr beurteilt?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nach &lt;strong&gt;objektiven Kriterien &lt;/strong&gt;aus der &lt;strong&gt;Sicht des Angegriffenen &lt;/strong&gt;unter &lt;strong&gt;Berücksichtigung aller Umstände des Einzelfalls&lt;/strong&gt;, aus der Sicht &lt;strong&gt;ex&lt;/strong&gt; &lt;strong&gt;ante &lt;/strong&gt;(vorher).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(226, 148, 20);"&gt;notwendige &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Verteidigung?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Notwendig ist jene Verteidigung, die unter den &lt;strong&gt;verfügbaren Mitteln &lt;/strong&gt;das &lt;strong&gt;schonendste &lt;/strong&gt;darstellt, um den &lt;strong&gt;Angriff sofort und endgültig abzuwehren.&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Welche Handlungen rechtfertigt die Notwehr?&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wie heißen überschießende Handlungen?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Gerechtfertigt ist immer nur die &lt;strong&gt;notwendige &lt;/strong&gt;Verteidigung.&lt;/li&gt;&lt;li&gt;Jede Überschreitung ist ein &lt;strong&gt;Handlungsexzess &lt;/strong&gt;(intensiv oder extensiv) und ist nicht rechtmäßig.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Auswirkung von &lt;strong&gt;Begleitwissen &lt;/strong&gt;auf den Tatbildirrtum?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ist dem Täter die &lt;strong&gt;Verwirklichung &lt;/strong&gt;eines bestimmten &lt;strong&gt;Tatbestandsmerkmals &lt;/strong&gt;zumindest &lt;strong&gt;latent bewusst&lt;/strong&gt;, scheidet Tatbildirrtum aus&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Rechtswidrigkeit eines Angriffs (Voraussetzung für Notwehr)?&lt;/p&gt;&lt;p&gt;Was ist der Umkehrschluss?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Ein Angriff ist &lt;strong&gt;rechtswidrig&lt;/strong&gt;, wenn &lt;strong&gt;kein RFG &lt;/strong&gt;vorliegt.&lt;/li&gt;&lt;li&gt;Umkehrschluss Liegt RFG vor: &lt;strong&gt;Keine&lt;/strong&gt; &lt;strong&gt;Notwehr&lt;/strong&gt;!&lt;/li&gt;&lt;li class="ql-indent-1"&gt;z.B.: Keine Notwehr gegen Notwehr&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die zeitlichen Schranken der Notwehr?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Der Angriff muss &lt;strong&gt;unmittelbar&lt;/strong&gt; &lt;strong&gt;drohen&lt;/strong&gt; (Versuchsnähe) oder &lt;strong&gt;gegenwärtig &lt;/strong&gt;sein.&lt;/li&gt;&lt;li&gt;Ist der Angriff &lt;strong&gt;abgewehrt&lt;/strong&gt;, &lt;strong&gt;aufgegeben &lt;/strong&gt;oder die &lt;strong&gt;Handlung&lt;/strong&gt; &lt;strong&gt;abgeschlossen &lt;/strong&gt;kommt Notwehr &lt;strong&gt;nicht &lt;/strong&gt;mehr in &lt;strong&gt;Betracht&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die 3 Grenzen der Notwehr?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Notwehrfähige Rechtsgüter&lt;/strong&gt;: Notwehr ist gem &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/3" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§&amp;nbsp;3 StGB&lt;/a&gt; auf bestimmte Rechtsgüter beschränkt.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Bagatellschwelle&lt;/strong&gt;: Rechtsgutsbeeinträchtigungen unter der Bagatellschwelle (Vordrängeln, Rempelln, verbale sexuelle Anmache, ...) sind keine Angriffe (Abwehr durch Worte ausreichend). &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Unklare Rollenverteilung&lt;/strong&gt;: Bei unklarer Rollenverteilung kann sich keiner der Kontrahenten auf Notwehr berufen ( z.B.: Streit geht allmählich in handgreifliche Auseinandersetzung über)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Abgrenzung für Angriffe bzw. was ist kein Angriff?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Verhaltensweise &lt;strong&gt;ohne Handlungsqualität &lt;/strong&gt;(insbesondere vis absoluta)&lt;/li&gt;&lt;li&gt;Tierattacken&lt;/li&gt;&lt;li&gt;Naturereignisse&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Kann fahrlässiges oder sogar schuldloses Verhalten ein Angriff sein?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ja, denn ein Angriff &lt;strong&gt;erfordert nicht&lt;/strong&gt; notwendigerweise &lt;strong&gt;gewolltes &lt;/strong&gt;oder &lt;strong&gt;aktives &lt;/strong&gt;Tun.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Muss für Notwehr ein Angriff tatsächlich vorliegen?&lt;/p&gt;&lt;p&gt;Wie muss das vorliegen beurteilt werden?&lt;/p&gt;&lt;p&gt;Reicht die irrtümliche Annahme des Vorliegens?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Der Angriff muss &lt;strong&gt;tatsächlich &lt;/strong&gt;vorliegen.&lt;/li&gt;&lt;li&gt;Die Beurteilung muss aus der Sicht &lt;strong&gt;ex ante &lt;/strong&gt;(vorher) und nach &lt;strong&gt;objektiven Kriterien &lt;/strong&gt;erfolgen.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Irrtümliche &lt;/strong&gt;Annahme &lt;strong&gt;reicht nicht aus&lt;/strong&gt;, kann aber statt Notwehr&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/8" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§&amp;nbsp;8 StGB&lt;/a&gt; begründen.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein Angriff?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Angriff ist jedes &lt;strong&gt;menschliche Verhalten&lt;/strong&gt;, das die &lt;strong&gt;Beeinträchtigung von&lt;/strong&gt; &lt;strong&gt;Rechtsgütern&lt;/strong&gt; befürchten lässt.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Notwehrsituation?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ein &lt;strong&gt;gegenwärtiger &lt;/strong&gt;oder &lt;strong&gt;unmittelbar&lt;/strong&gt; &lt;strong&gt;drohender&lt;/strong&gt; &lt;strong&gt;rechtswidriger Angriff &lt;/strong&gt;auf ein &lt;strong&gt;notwehrfähiges Rechtsgut&lt;/strong&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Rechtsgrundlage für Notwehr?&lt;/p&gt;&lt;p&gt;Was sind die drei prinzipiellen Bauelemente des RFG Notwehr?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/3" rel="noopener noreferrer" target="_blank"&gt;§&amp;nbsp;3 StGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Notwehr&lt;strong&gt;situation&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Notwehr&lt;strong&gt;handlung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(226, 148, 20);"&gt;subjektives&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;Rechtfertigungs&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(226, 148, 20);"&gt;element&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die drei prinzipiellen Bauelemente (Strukturelemente) eines RFG?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Rechtfertigungs&lt;strong&gt;situation&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Rechtfertigungs&lt;strong&gt;handlung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;subjektives&lt;/strong&gt; Rechtfertigungs&lt;strong&gt;element&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wofür steht RFG?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Rechtfertigungsgrund&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie wirkt der &lt;strong&gt;Tatbildirrtum&lt;/strong&gt;, und warum wird er restriktiv gehandhabt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Durch den &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Tatbildirrtum &lt;/span&gt;&lt;strong&gt;entfällt &lt;/strong&gt;der &lt;strong&gt;Tatvorsatz&lt;/strong&gt;, da die &lt;strong&gt;Wissenskomponente&lt;/strong&gt; entfällt.&lt;/li&gt;&lt;li&gt;Der Tatbildirrtum hat daher &lt;strong&gt;täterfreundliche Konsequenzen&lt;/strong&gt;, darum wird er restriktiv gehandhabt.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Sonderregelung für Irrtum im Bereich der Umweltdelikte?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;gem &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/183a" rel="noopener noreferrer" target="_blank"&gt;§ 183a StGB&lt;/a&gt; Haftung nach dem Vorsatzdelikt bei &lt;strong&gt;Vorwerfbarkeit &lt;/strong&gt;des Irrtums&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist Irrtum über &lt;/span&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(226, 148, 20);"&gt;Blankettmerkmale&lt;/span&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Blankettmerkmale sind &lt;strong&gt;normative &lt;/strong&gt;Tatbestandsmerkmale, es ist also eine Form des Irrtums über normative Merkmale.&lt;/li&gt;&lt;li&gt;Täter kann häufig den&lt;strong&gt; sozialen und rechtlichen Bedeutungsgehalt&lt;/strong&gt; nicht einmal nach Laienart erkennen, daher&lt;strong&gt; entfällt der Tatvorsatz &lt;/strong&gt;(Fahrlässigkeit sofern Delikt vorhanden, sonst Freispruch)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was sind Blankettmerkmale bzw ein Blankettstrafgesetz?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Ein strafrechtliches Delikt verweist zur &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Beschreibung eines strafbaren Verhaltens&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; (ganz oder teilweise) auf &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;andere Vorschriften&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist Irrtum über &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Schuldmerkmale&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Subjektive Schuldmerkmale &lt;/strong&gt;wirken auch &lt;strong&gt;privilegierend&lt;/strong&gt;, wenn die &lt;strong&gt;deliktspezifische Gemütsverfassung &lt;/strong&gt;durch eine &lt;strong&gt;falsche Einschätzung&lt;/strong&gt; der tatsächlichen Umstände ausgelöst wird (z.B.: &lt;strong&gt;Affekt zur Tötung&lt;/strong&gt; gem §&amp;nbsp;76 StgB wird auch erfüllt, wenn der Affekt durch falsche Nachricht ausgelöst wird)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist Irrtum über &lt;strong style="color: rgb(226, 148, 20); background-color: rgba(0, 0, 0, 0);"&gt;privilegierende &lt;/strong&gt;Tatbestandsmerkmale?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage für die Abänderung Strafe?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Glaubt der Täter irrtümlich, ein &lt;strong&gt;privilegierendes &lt;/strong&gt;Tatbestandsmerkmal zu erfüllen, so lädt er &lt;strong&gt;subjektiv nur die geringere Schuld des privilegierten Delikts &lt;/strong&gt;auf sich, und ist gem. &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/4" rel="noopener noreferrer" target="_blank"&gt;§&amp;nbsp;4 StGB&lt;/a&gt; nur nach diesem zu Strafen &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist Irrtum über &lt;strong&gt;qualifizierende &lt;/strong&gt;Tatbestandsmerkmale?&lt;/p&gt;&lt;p&gt;Was ist die Ausnahme?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Verkennt der Täter das Vorliegen eines &lt;strong&gt;qualifizierenden Tatbestandsmerkmals&lt;/strong&gt;, haftet er nur im Rahmen des &lt;strong&gt;Grunddelikts&lt;/strong&gt;. &lt;/li&gt;&lt;li&gt;Ausnahme: Irrtum über &lt;strong&gt;Wertqualifikationen &lt;/strong&gt;(Vermögensdelikte) wird in der Praxis umgekehrt gehandhabt (Dieb erwartet größtmögliche Beute)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist dolus generalis?&lt;/p&gt;&lt;p&gt;Was ist die herrschende Ansicht dazu?&lt;/p&gt;&lt;p&gt;Welche Arten gibt es, und wie wirken Sie sich auf die Strafbarkeit aus?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Die ganze Tat umfassender "genereller Vorsatz"&lt;/li&gt;&lt;li&gt;Heute überholt, hA sieht einen &lt;strong&gt;Sonderfall des Irrtums über den Kausalverlauf &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Folgen (bei Änderung des Kausalverlaufs):&lt;/li&gt;&lt;li class="ql-indent-1"&gt;bei &lt;strong&gt;unwesentlicher &lt;/strong&gt;Änderung: Strafbarkeit für das &lt;strong&gt;vollendete Delikt.&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;z.B.: Täter wirft vermeintlich bereits getötetes Opfer in Fluss, Tod tritt erst durch Ertrinken ein. → Vollendeter Mord.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;bei &lt;strong&gt;wesentlicher &lt;/strong&gt;Änderung: Strafbarkeit wegen &lt;strong&gt;Versuchs&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;z.B.: Vermeintlich bereits getötetes Opfer ist im Kofferraum und stirbt erst durch Auffahrunfall → versuchter Mord.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist aberratio ictus? &lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Welche Arten gibt es, und begründen sie Tatbildirrtum?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Infolge von &lt;strong&gt;Abirren &lt;/strong&gt;(Fehlgehen) &lt;strong&gt;des&lt;/strong&gt; &lt;strong&gt;Angriffs &lt;/strong&gt;wird ein &lt;strong&gt;anderes als das anvisierte Objekt&lt;/strong&gt; (oder Person) getroffen.&lt;/li&gt;&lt;li&gt;sowohl bei gleichartigem als auch ungleichartigem Objekt ist &lt;strong&gt;Versuch hinsichtlich des gewollten Erfolgs&lt;/strong&gt; und unter Umständen &lt;strong&gt;fahrlässige Tat in Bezug auf tatsächlich eingetretenen Erfolg&lt;/strong&gt; anzunehmen → kein Entfall der Strafbarkeit aufgrund von Tatbildirrtum.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Irrtum über das Tatobjekt (Objektsirrtum)?&lt;/p&gt;&lt;p&gt;Welche Arten gibt es, und begründen sie Tatbildirrtum?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Täter &lt;strong&gt;irrt &lt;/strong&gt;sich über die &lt;strong&gt;Identität &lt;/strong&gt;(oder sonstige &lt;strong&gt;delkitsrelevante&lt;/strong&gt; &lt;strong&gt;Eigenschaften&lt;/strong&gt;) einer Person oder Sache.&lt;/li&gt;&lt;li&gt;Arten: Irrtum über:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;gleichartiges &lt;/strong&gt;Tatobjekt (Mensch - Mensch): Berührt den Tatvorsatz nicht, daher &lt;strong&gt;kein Tatbildirrtum&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;ungleichartiges &lt;/strong&gt;Tatobjekt (Mensch - Wachsfigur): &lt;strong&gt;Tatbildirrtum &lt;/strong&gt;der Tatvorsatz ausschließt.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Bestrafung ist trotz Tatbildirrtum möglich?&lt;/p&gt;&lt;p&gt;Was sind die Voraussetzungen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Bestrafung wegen &lt;strong&gt;fahrlässiger &lt;/strong&gt;Tat.&lt;/li&gt;&lt;li&gt;Es gibt ein &lt;strong&gt;entsprechendes Fahrlässigkeitsdelikt&lt;/strong&gt;, und der &lt;strong&gt;Irrtum beruht auf Fahrlässigkeit&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Was ist der Tatbildirrtum über &lt;/span&gt;&lt;strong style="color: rgb(226, 148, 20); background-color: rgb(40, 45, 88);"&gt;Wertqualifikation&lt;/strong&gt;&lt;span style="color: rgb(226, 148, 20); background-color: rgb(40, 45, 88);"&gt;?&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Welche Beschränkung gibt es?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Die &lt;strong&gt;Wertqualifikationen&lt;/strong&gt; &lt;strong&gt;der Vermögensdelikte&lt;/strong&gt; sind echte TB-Merkmale und müssen vom &lt;strong&gt;Tatvorsatz mitumfasst&lt;/strong&gt; sein.&lt;/li&gt;&lt;li&gt;Tatbildirrtum scheitert idR aber mit dem Hinweis, dass &lt;strong&gt;jeder Dieb eine möglichst hohe Beute erwartet&lt;/strong&gt;, und damit hinsichtlich &lt;strong&gt;Wertqualifikation &lt;/strong&gt;jedenfalls mit &lt;strong&gt;dolus&lt;/strong&gt; &lt;strong&gt;eventualis &lt;/strong&gt;handelt.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Was der Tatbildirrtum über &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Kausalverlauf&lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;?&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Welche Beschränkung gibt es?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Der Tatvorsatz muss den &lt;strong&gt;Kausalverlauf &lt;/strong&gt;nur in &lt;strong&gt;wesentlichen Zügen &lt;/strong&gt;umfassen.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Unwesentliche&lt;/strong&gt; &lt;strong&gt;Abweichungen &lt;/strong&gt;stellen daher keinen Tatbildirrtum dar.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Was ist der Tatbildirrtum &lt;/span&gt;über &lt;strong style="color: rgb(226, 148, 20); background-color: rgba(0, 0, 0, 0);"&gt;normative &lt;/strong&gt;&lt;span style="color: rgb(226, 148, 20); background-color: rgba(0, 0, 0, 0);"&gt;TB&lt;/span&gt;-&lt;span style="color: rgb(226, 148, 20); background-color: rgba(0, 0, 0, 0);"&gt;Merkmale?&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="color: rgb(226, 148, 20); background-color: rgba(0, 0, 0, 0);"&gt;Welche Beschränkung gibt es?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Tatbildirrtum liegt vor, wenn der Täter die dem &lt;strong&gt;normativen Begriff&lt;/strong&gt; zugrunde liegenden &lt;strong&gt;tatsächlichen Umstände nicht wahrgenommen&lt;/strong&gt; oder den&lt;strong&gt; sozialen und rechtlichen Bedeutungsgehalt nicht erkannt &lt;/strong&gt;hat.&lt;/li&gt;&lt;li&gt;Ist die&lt;strong&gt; laienmäßige Einschätzung &lt;/strong&gt;durch den Täter aber zumindest&lt;strong&gt; parallel zu jener des Rechts&lt;/strong&gt;, scheidet Tatbildirrtum aus.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Arten des Tatbildirrtums gibt es?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Irrtum über &lt;strong&gt;normative TB&lt;/strong&gt;-&lt;strong&gt;Merkmale&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Irrtum über &lt;strong&gt;Kausalverlauf&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Irrtum über &lt;strong&gt;Wertqualifikation&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann liegt &lt;strong&gt;Tatbildirrtum&lt;/strong&gt; vor?&lt;/p&gt;&lt;p&gt;Was reicht aus, damit ein Tatbildirrtum vorliegt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Wenn der Täter nicht erkennt, dass er einen &lt;strong&gt;Sachverhalt verwirklicht&lt;/strong&gt;, der einem &lt;strong&gt;gesetzlichen Tatbild&lt;/strong&gt; entspricht.&lt;/li&gt;&lt;li&gt;Es reicht aus, wenn sich der Täter über &lt;strong&gt;eines von mehreren Tatbestandsmerkmalen&lt;/strong&gt; irrt.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein zentrales Element des objektiven Tatbestands?&lt;/p&gt;&lt;p&gt;Ist dieses üblicherweise geschrieben oder ungeschrieben?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Kausalität&lt;/strong&gt;. Wird im Gesetz nur ausnahmsweise angesprochen, zählt normalerweise zu den &lt;strong&gt;ungeschriebenen &lt;/strong&gt;Merkmalen.&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Was ist das Problem des &lt;strong&gt;Vorsatzes trotz Schuldunfähigkeit&lt;/strong&gt;?&lt;/p&gt;</t>
   </si>
   <si>
@@ -73,7 +349,7 @@
     <t>&lt;p&gt;Der Täter muss die &lt;strong&gt;Verwirklichung &lt;/strong&gt;des &lt;strong&gt;Tatbildes wollen&lt;/strong&gt;, und sich zumindest mit der &lt;strong&gt;Verletzung &lt;/strong&gt;des &lt;strong&gt;Rechtsguts abfinden&lt;/strong&gt;.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Wie Verhält sich der Vorsatz um Kausalverlauf?&lt;/p&gt;&lt;p&gt;Wie sieht die hL dies im Detail?&lt;/p&gt;</t>
+    <t>&lt;p&gt;Wie Verhält sich der Vorsatz zum Kausalverlauf?&lt;/p&gt;&lt;p&gt;Wie sieht die hL dies im Detail?&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;ul&gt;&lt;li&gt;Vorsatz muss sich auch auf den &lt;strong&gt;Kausalverlauf &lt;/strong&gt;(Teil des objektiven Tatbestands) &lt;strong&gt;beziehen&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;hl sagt: Kenntnis des Kausalverlaufs in &lt;strong&gt;wesentlichen Zügen&lt;/strong&gt; &lt;strong&gt;genügt&lt;/strong&gt;, Kenntnis der &lt;strong&gt;Einzelheiten nicht erfordert&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
@@ -100,7 +376,7 @@
     <t>&lt;p&gt;Was umfasst die Wissenskomponente?&lt;/p&gt;&lt;p&gt;Was ist die Mindestanforderung an Wissen? &lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;ul&gt;&lt;li&gt;Kenntnis aller Tatsachen, auf welche sich der objektive Tatbestand bezieht.&lt;/li&gt;&lt;li&gt;Bereits &lt;strong&gt;undeutliche &lt;/strong&gt;und &lt;strong&gt;unreflektierte Vorstellungen &lt;/strong&gt;genügen den Anforderungen des Wissens&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;ul&gt;&lt;li&gt;Kenntnis &lt;strong&gt;aller Tatsachen&lt;/strong&gt;, auf welche sich der &lt;strong&gt;objektive Tatbestand &lt;/strong&gt;bezieht.&lt;/li&gt;&lt;li&gt;Bereits &lt;strong&gt;undeutliche &lt;/strong&gt;und &lt;strong&gt;unreflektierte Vorstellungen &lt;/strong&gt;genügen den Anforderungen des Wissens&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Aus welchen 2 Komponenten besteht der Vorsatz?&lt;/p&gt;&lt;p&gt;Wie sind diese in der Legaldefinition geregelt?&lt;/p&gt;</t>
@@ -115,16 +391,10 @@
     <t>&lt;ul&gt;&lt;li&gt;Tathandlung&lt;/li&gt;&lt;li&gt;Tatobjekt&lt;/li&gt;&lt;li&gt;allfällige Tatmodalitäten&lt;/li&gt;&lt;li&gt;Erfolg&lt;/li&gt;&lt;li&gt;Kausalverlauf in groben Zügen&lt;/li&gt;&lt;li&gt;etwaige Deliktsqualifikationen (z.B.: Wertqualifikationen)&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Welche Stufen des Vorsatzes gibt es?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ol&gt;&lt;li&gt;Bedingter Vorsatz&lt;/li&gt;&lt;li&gt;Absicht&lt;/li&gt;&lt;li&gt;Wissentlichkeit&lt;/li&gt;&lt;/ol&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was ist eine vorsätzliche Handlung?&lt;/p&gt;&lt;p&gt;Was ist die gesetzliche Grundlage?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Vorsätzlich handelt, wer einen Sachverhalt verwirklichen will, der einem geseztlichen Tatbild entspricht (&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/5" rel="noopener noreferrer" target="_blank"&gt;§ 5 Abs 1 StGB&lt;/a&gt;)&lt;/p&gt;</t>
+    <t>&lt;p&gt;Vorsätzlich handelt, wer einen &lt;strong&gt;Sachverhalt verwirklichen will&lt;/strong&gt;, der einem &lt;strong&gt;gesetzlichen Tatbild &lt;/strong&gt;entspricht (&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/5" rel="noopener noreferrer" target="_blank"&gt;§ 5 Abs 1 StGB&lt;/a&gt;)&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was ist der objektive Tatbestand?&lt;/p&gt;&lt;p&gt;Wie wird er noch bezeichnet?&lt;/p&gt;&lt;p&gt;Was umfasst er?&lt;/p&gt;</t>
@@ -139,10 +409,10 @@
     <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Kausalität&lt;/strong&gt;: es geht darum, ob eine bestimmte Handlung einen bestimmten Erfolg verursacht hat.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Hat weder Wertung noch Vorwurf&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Schuld&lt;/strong&gt;: es geht darum, ob dem Täter der verursachte Erfolg auch rechtlich vorgeworfen werden kann.&lt;/li&gt;&lt;li&gt;Kausalität ist vor Schuld zu prüfen. Mit Verneinung der Kausalität erübrigt sich die Schuldfrage.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist die objektive Zurechenbarkeit?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Der Erfolg ist in spezifisch normativer Weise mit der Handlung verknüpft&lt;/p&gt;</t>
+    <t>&lt;p&gt;Was ist die objektive Zurechenbarkeit des Erfolgs?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der Erfolg ist in &lt;strong&gt;spezifisch normativer Weise&lt;/strong&gt; mit der Handlung verknüpft&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was ist überholende Kausalität?&lt;/p&gt;</t>
@@ -181,7 +451,7 @@
     <t>&lt;p&gt;Der &lt;strong&gt;wirkliche &lt;/strong&gt;Geschehensablauf und Erfolg in seiner &lt;strong&gt;konkreten &lt;/strong&gt;Gestalt. Hypothetische Verläufe bleiben außer Betracht.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist die Äquivalenztheorie?&lt;/p&gt;</t>
+    <t>&lt;p&gt;Was ist die Äquivalenztheorie der Kausalität?&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Ein Tun ist &lt;strong&gt;kausal &lt;/strong&gt;für einen &lt;strong&gt;Erfolg&lt;/strong&gt;, wenn es &lt;strong&gt;nicht weggedacht &lt;/strong&gt;werden kann, ohne dass der &lt;strong&gt;Erfolg &lt;/strong&gt;in seiner konkreten Gestalt &lt;strong&gt;entfällt&lt;/strong&gt;.&lt;/p&gt;</t>
@@ -211,12 +481,6 @@
     <t>&lt;p&gt;Die Tathandlung&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist ein zentrales Element des objektiven Tatbestands davon?&lt;/p&gt;&lt;p&gt;Ist dieses üblicherweise geschrieben oder ungeschrieben?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Kausalität&lt;/strong&gt;. Wird im Gesetz nur ausnahmsweise angesprochen, zählt normalerweise zu den &lt;strong&gt;ungeschriebenen &lt;/strong&gt;Merkmalen.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Was sind &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;normative &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Tatbestandselemente?&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
@@ -461,12 +725,6 @@
   </si>
   <si>
     <t>&lt;ul&gt;&lt;li&gt;Sie beseitigen nicht die &lt;strong&gt;Tatbestandsmäßigkeit&lt;/strong&gt;, sondern nur das &lt;strong&gt;Unrecht&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;Die Handlung wird von der Rechtsordnung gebilligt, es darf keine Strafe oder vorbeugende Maßnahme verhängt werden. &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wofür steht RFG?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Rechtfertigungsgrund&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was ist das Regel-Ausnahme-Prinzip?&lt;/p&gt;</t>
@@ -1108,7 +1366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B118"/>
+  <dimension ref="A1:B161"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -2058,6 +2316,350 @@
         <v>235</v>
       </c>
     </row>
+    <row r="119" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Add cards for chapters 19,20,21,22,23
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - VU Strafrecht I - 1. Klausur (JKU, Austria).xlsx
+++ b/flashcards/Memcode - VU Strafrecht I - 1. Klausur (JKU, Austria).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="519">
   <si>
     <t>Question</t>
   </si>
@@ -19,12 +19,396 @@
     <t>Answer</t>
   </si>
   <si>
+    <t>&lt;p&gt;Wann ist der Versuch strafbar?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Gem &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/15" rel="noopener noreferrer" target="_blank"&gt;§ 15 (2) StGB&lt;/a&gt; ist der Versuch bei allen Vorsatzdelikten strafbar.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Strafausschließungsgründe?&lt;/p&gt;&lt;p&gt;Was ist die wichtigste Rechtsgrundlage im Gerichtsalltag? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Umstände, die idR schon &lt;strong&gt;bei &lt;/strong&gt;der &lt;strong&gt;Begehung &lt;/strong&gt;der Straftat &lt;strong&gt;vorliegen &lt;/strong&gt;und einer &lt;strong&gt;Bestrafung &lt;/strong&gt;des Täters &lt;strong&gt;entgegenstehen&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;§ 88 (2) StGB&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Verjährung?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/57" rel="noopener noreferrer" target="_blank"&gt;§§ 57 f StGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;mutmaßlicher Täter kann nach &lt;strong&gt;Ablauf einer gewissen Zeit&lt;/strong&gt; nicht mehr verfolgt werden - &lt;strong&gt;Strafbarkeit entfällt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welcher Art von Rücktritt entspricht die &lt;strong&gt;tätige&lt;/strong&gt; Reue?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage für die tätige Reue? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Rücktritt vom &lt;strong&gt;versuchten&lt;/strong&gt; Delikt&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/167" rel="noopener noreferrer" target="_blank"&gt;§ 167 StGB&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Was bedeutet &lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;verwirkt&lt;/strong&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt; &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;im Gesetzestext?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Fällig - die verwirkte Strafe ist die &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;fällige &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Strafe&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Strafaufhebungsgründe?&lt;/p&gt;&lt;p&gt;Was sind die 2 wichtigsten und deren Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Voraussetzungen unter denen die wegen einer Straftat bereits verwirkte (&lt;strong&gt;fällige&lt;/strong&gt;) &lt;strong&gt;Strafe &lt;/strong&gt;wieder &lt;strong&gt;aufgehoben &lt;/strong&gt;wird.&lt;/li&gt;&lt;li&gt;Rücktritt vom Versuch ( &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/16" rel="noopener noreferrer" target="_blank"&gt;§ 16&lt;/a&gt; ) und tätige Reue ( &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/167" rel="noopener noreferrer" target="_blank"&gt;§ 167&lt;/a&gt; )&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein qualifizierter Versuch? &lt;/p&gt;&lt;p&gt;Was ist die Folge hinsichtlich Rücktritt?&lt;/p&gt;&lt;p&gt;Beispiele?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Ein Versuch, in dem ein &lt;strong&gt;vollendetes Delikt enthalten &lt;/strong&gt;ist&lt;/li&gt;&lt;li&gt;Das im Versuch &lt;strong&gt;enthaltene Delikt &lt;/strong&gt;bleibt vom Rücktritt unberührt und daher &lt;strong&gt;strafbar&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;z.B.: Rücktritt von versuchtem Mord: Bestrafung wegen Körperverletzung&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Putativrücktritt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/16" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(115, 133, 197);"&gt;§ 16 (2) StGB&lt;/a&gt;: Erfolg bleibt &lt;strong&gt;ohne Zutun des Täters aus&lt;/strong&gt;, er ist sich dessen aber &lt;strong&gt;nicht bewusst &lt;/strong&gt;und nimmt &lt;strong&gt;ernstlich bemüht &lt;/strong&gt;einen &lt;strong&gt;Rücktritt &lt;/strong&gt;vor.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein fehlgeschlagener Versuch?&lt;/p&gt;&lt;p&gt;Was sind die Rechtsfolgen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Versuch ist fehlgeschlagen, wenn der Täter &lt;strong&gt;erkennt oder&lt;/strong&gt; &lt;strong&gt;glaubt&lt;/strong&gt;, dass sein er &lt;strong&gt;Ziel nicht mehr erreichen&lt;/strong&gt; kann (oder einen neuen Versuch bentigt)&lt;/li&gt;&lt;li&gt;Folgen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;kein Rücktritt oder Putativrücktritt möglich&lt;/li&gt;&lt;li class="ql-indent-1"&gt;also VOR Rücktritt zu prüfen.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was sind die 3 Voraussetzungen für den Rücktritt vom &lt;/span&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;beendeten &lt;/span&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Versuch?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Abwendung&lt;/strong&gt; des Erfolgs:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Strenge Anforderung: Erfolg muss &lt;strong&gt;tatsächlich &lt;/strong&gt;abgewendet werden.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Freiwilligkeit&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;Frank&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;'sche und&lt;/span&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt; &lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;Roxin&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;'sche Formel &lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;eigenes Zutun &lt;/strong&gt;des Täters:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;aktives&lt;/strong&gt; Gegensteuern durch gefahrneutralisierendes Handeln&lt;/li&gt;&lt;li class="ql-indent-1"&gt;passiv oder versehen &lt;strong&gt;reicht nicht&lt;/strong&gt;!&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Erfolg tritt trotz freiwilligem Rücktritt ein &lt;/p&gt;&lt;ul&gt;&lt;li&gt;Welche Folgen kann es geben?&lt;/li&gt;&lt;li&gt;Wie ist dieser Fall zu beurteilen?&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Straflos wegen Rücktritt oder Strafbar wegen vollendetem Delikt&lt;/li&gt;&lt;li&gt;Maßgeblich ist, ob der &lt;strong&gt;Eintritt des Erfolgs&lt;/strong&gt; nach Adäquanz- und Risikozusammmehang noch &lt;strong&gt;objektiv zugeordnet &lt;/strong&gt;werden kann&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die Roxin'sche Formel für die Freiwilligkeit?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Der Rücktritt ist &lt;strong&gt;unfreiwillig&lt;/strong&gt;, wenn die Tat zwar objektiv noch ausführbar ist (oder der Täter sie für ausführbar hält), es aber &lt;strong&gt;iSd Verbrechervernunft unklug &lt;/strong&gt;wäre (angesichts der veränderten Umstände)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Frank'sche Formel für die Freiwilligkeit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;psychologischer Ansatz, deckt&lt;strong&gt; nicht alle Fälle&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;"ich will nicht, obwohl ich kann"&lt;/li&gt;&lt;li&gt;Entscheidend ist, dass der &lt;strong&gt;Täter &lt;/strong&gt;(trotz veränderter Umstände) die &lt;strong&gt;Vorstellung &lt;/strong&gt;hat, dass eine seinem Tatplan entsprechende &lt;strong&gt;Vollendung noch möglich &lt;/strong&gt;wäre.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die 2 Voraussetzungen für den Rücktritt vom &lt;strong&gt;unbeendeten &lt;/strong&gt;Versuch?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Endgültige &lt;/strong&gt;Aufgabe der Tatausführung: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Abbruch durch bloßes &lt;strong&gt;Nichtweiterhandeln &lt;/strong&gt;genügt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;endgültig: Täter &lt;strong&gt;verzichtet&lt;/strong&gt; auf &lt;strong&gt;weitere Ausführung&lt;/strong&gt;, bloße Unterbrechung reicht nicht&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Freiwilligkeit&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Frank&lt;/strong&gt;'sche und&lt;strong&gt; Roxin&lt;/strong&gt;'sche Formel (oft deckungsgleich, aber gut beide zur Gegenkontrolle zu verwenden) &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die 2 Arten des Rücktritts?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;einfacher &lt;/strong&gt;Rücktritt: vom &lt;strong&gt;unbeendeten &lt;/strong&gt;Versuch&lt;/li&gt;&lt;li&gt;&lt;strong&gt;tätiger &lt;/strong&gt;Rücktritt: vom &lt;strong&gt;beendeten &lt;/strong&gt;Versuch&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Rücktritt des Alleintäters? &lt;/p&gt;&lt;p&gt;Was ist die Rechtsfolge?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Täter &lt;strong&gt;gibt die Tatausführung freiwillig au&lt;/strong&gt;f bzw bewirkt, dass die Tat nicht vollendet wird.&lt;/li&gt;&lt;li&gt;Folge: volle Straffreiheit&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/16" rel="noopener noreferrer" target="_blank"&gt;§ 16 StGB&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Stellt das Beenden eines Versuchs einen Rücktritt nach § 16 dar?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nein, dafür müsste die &lt;strong&gt;Gefahr neutralisiert &lt;/strong&gt;werden ( gefahrneutralisierendes Handeln )&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann ist ein Versuch beendet, wann nicht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Der Versuch ist beendet, wenn der &lt;strong&gt;Täter glaubt&lt;/strong&gt;, alles zur &lt;strong&gt;Vollendung&lt;/strong&gt; der Tat &lt;strong&gt;Erforderliche&lt;/strong&gt; &lt;strong&gt;getan&lt;/strong&gt; zu haben. &lt;/li&gt;&lt;li&gt;Glaubt er dagegen, noch &lt;strong&gt;weiterhandeln &lt;/strong&gt;zu müssen, ist der Versuch &lt;strong&gt;unbeendet&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Fallprüfungsschema für den Tatbestand des Versuchs?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Nichterfüllung des gesetzlichen Tatbildes&lt;/strong&gt;: es dürfen nicht sämtliche objektiven Tatbestandmerkmale erfüllt sein&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Voller Tatentschluss&lt;/strong&gt;: Täter muss mit vollem Tatentschluss handeln (meist identisch mit Tatvorsatz)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ausführungshandlung bzw. ausführungsnahe Handlung&lt;/strong&gt;: sonst bloße Vorbereitungshandlung.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Tatbestand des &lt;strong&gt;versuchten Delikts&lt;/strong&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Vollständige Tat Versucht&lt;/li&gt;&lt;li&gt;Aber vor Vollendung "steckengeblieben"&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann ist ein Delikt vollendet?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sobald alle Tatbestandsmerkmale erfüllt sind&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Abgrenzung zwischen Vorbereitung und &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Versuch&lt;/span&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der Versuch beginnt mit der Tätigung einer &lt;strong&gt;ausführungsnahen Handlung&lt;/strong&gt;.&lt;/p&gt;&lt;p&gt;Jedenfalls ist der Versuch anzunehmen, wenn eine &lt;strong&gt;Ausführungshandlung &lt;/strong&gt;vorgenommen wird.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Verhältnis zwischen &lt;strong&gt;Verbotsirrtum &lt;/strong&gt;und &lt;strong&gt;Tatbildirrtum&lt;/strong&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Tatbildirrtum&lt;/strong&gt;: Der Täter erkennt nicht, dass er einen Sachverhalt verwirklicht, der einem gesetzlichen Tatbild entspricht &lt;/li&gt;&lt;li class="ql-indent-1"&gt;bezieht sich also auf die &lt;strong&gt;tatsächliche &lt;/strong&gt;Seite&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verbotsirrtum&lt;/strong&gt;: Täter kennt Sachverhalt, weis aber nicht über das Unrecht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;bezieht sich also auf die &lt;strong&gt;rechtliche &lt;/strong&gt;Seite&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie verhält sich der &lt;strong&gt;vorwerfbare Verbotsirrtum &lt;/strong&gt;zum &lt;strong&gt;potenziellen&lt;/strong&gt; &lt;strong&gt;Unrechtsbewusstsein&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Synonym&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Beide bringen zum Ausdruck, dass der Täter das &lt;strong&gt;Unrecht nicht&lt;/strong&gt; &lt;strong&gt;erkannt &lt;/strong&gt;hat, aber sich hätte &lt;strong&gt;erkundigen müssen&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ist Verbotsirrtum in der Praxis im Regelfall vorwerfbar oder nicht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Im Regelfall vorwerfbar → Schuld und Strafbarkeit bleiben bestehen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Rechtsfolgen des Verbotsirrtums?&lt;/p&gt;&lt;p&gt;Was ist die Voraussetzung für den Eintritt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Schuld und damit Strafe werden ausgeschlossen (&lt;strong&gt;Schuldausschließungsgrund&lt;/strong&gt;)&lt;/li&gt;&lt;li&gt;Voraussetzung: Verbotsirrtum muss &lt;strong&gt;nic&lt;span class="ql-cursor"&gt;﻿&lt;/span&gt;ht vorwerfbar &lt;/strong&gt;sein.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie wird der Verbotsirrtum in der Praxis gehandhabt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Geht meist ins Leere da bereits &lt;strong&gt;latentes &lt;/strong&gt;oder &lt;strong&gt;laienmäßiges Unrechtsbewusstsein &lt;/strong&gt;Verbotsirrtum ausschließt&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die zwei Arten des Verbotsirtums?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;direkter &lt;/strong&gt;Verbotsirrtum: Täter &lt;strong&gt;erkennt nicht&lt;/strong&gt;, dass seine Tat verboten/unrecht ist&lt;/li&gt;&lt;li&gt;&lt;strong&gt;indirekter &lt;/strong&gt;Verbotsirrtum: Täter &lt;strong&gt;irrt über&lt;/strong&gt; Existenz/Grenzen eines &lt;strong&gt;Rechtfertigungsgrundes &lt;/strong&gt;-&amp;gt; er weiß, dass die Tat verboten ist, denkt aber sie er darf sie ausnahmsweise begehen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie heißt der Verbotsirrtum im StGB (&lt;strong&gt;Rechtsgrundlage&lt;/strong&gt;)?&lt;/p&gt;&lt;p&gt;Warum wird der Begriff Verbotsirrtum im Schrifttum bevorzugt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Rechtsirrtum gem &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/9" rel="noopener noreferrer" target="_blank"&gt;§ 9 StGB&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Verbotsirrtum?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der Täter &lt;strong&gt;erkennt das Unrecht seiner Tat nicht&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;-&amp;gt; Umkehr des Unrechtsbewusstseins&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Verhältnis zwischen Unrechtsbewusstsein und Tatvorsatz?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Vorsatz&lt;/strong&gt;: bezieht sich auf &lt;strong&gt;tatsächliche Seite &lt;/strong&gt;der Tat&lt;/li&gt;&lt;li class="ql-indent-1"&gt;muss &lt;strong&gt;tatsächlich vorhanden &lt;/strong&gt;sein.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Unrechtsbewusstsein&lt;/strong&gt;: bezieht sich auf die rechtliche Seite (Bewertung der Tat als Unrecht)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;muss nur &lt;strong&gt;potenziell vorhanden &lt;/strong&gt;sein.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Was ist die Folge von Handlungen ohne aktuellem und potenziellem Unrechtsbewusstsein?&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Schuld entfällt&lt;/p&gt;</t>
   </si>
   <si>
+    <t>&lt;p&gt;Was ist potenzielles Unrechtsbewusstsein?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Vorwerfbarer Mangel &lt;/strong&gt;des Unrechtsbewusstseins&lt;/li&gt;&lt;li&gt;Der Täter &lt;strong&gt;erkennt &lt;/strong&gt;das &lt;strong&gt;Unrecht&lt;/strong&gt; der Tat &lt;strong&gt;nicht&lt;/strong&gt;, wäre aber &lt;strong&gt;verpflichtet &lt;/strong&gt;gewesen sich danach &lt;strong&gt;zu erkundigen&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist aktuelles Unrechtsbewusstsein?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Zur Zeit der tat &lt;strong&gt;wirklich vorhandenes &lt;/strong&gt;Unrechtsbewusstsein.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Unrechtsbewusstsein? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Das Bewusstsein, dass die Tat gegen die Rechtsordnung verstößt.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Unterschied zwischen alic und § 287 (1) StGB&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Erfüllen &lt;strong&gt;ähnliche Funktionen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;alic&lt;/strong&gt;: Vorsatz/Fahrlässigkeit bezieht sich auf die konkrete rechtswidrige Tat&lt;/li&gt;&lt;li&gt;&lt;strong&gt;287 (1)&lt;/strong&gt;: bestraft, wer die im Rausch begangenen Tat &lt;strong&gt;weder gewollt noch vorausgesehen hat&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie funktioniert die Schuldprüfung bei &lt;strong&gt;alic&lt;/strong&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Schuldprüfung wird auf den &lt;strong&gt;Zeitpunkt&lt;/strong&gt; &lt;strong&gt;verlegt&lt;/strong&gt;, in dem sich der Täter &lt;strong&gt;in den Zustand der Schuldunfähigkeit versetzt hat&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(226, 148, 20);"&gt;fahrlässige &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;actio libera in causa?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Täter versetzt sich in einen die Schuldfähigkeit ausschließenden Rauschzustand, obwohl er &lt;strong&gt;voraussehen hätte müssen&lt;/strong&gt;, dass er in diesem Zustand ein &lt;strong&gt;bestimmtes Delikt begehen wird.&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die &lt;strong&gt;vorsätzliche &lt;/strong&gt;actio libera in causa?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Täter hat sich mit dem &lt;strong&gt;Vorsatz &lt;/strong&gt;in den Status der Schuldunfähigkeit versetzt, in diesem&lt;strong&gt; Zustand eine rechtswidrige Tat zu begehen.&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wofür steht &lt;strong&gt;alic&lt;/strong&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Actio libera in causa&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die &lt;strong&gt;partielle &lt;/strong&gt;Schuld&lt;strong&gt;unfähigkeit&lt;/strong&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Schuldunfähigkeit trifft nur &lt;strong&gt;Teile des Unrechts&lt;/strong&gt;, d.h. § 11 wird n&lt;strong&gt;ur für manche Delikte&lt;/strong&gt; angewandt.&lt;/li&gt;&lt;li&gt;z.B.: Schuldunfähig für krankheitsspezifische Straftaten, für alles andere aber voll Schuldfähig&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die &lt;strong&gt;verminderte &lt;/strong&gt;Schuld&lt;strong&gt;fähigkeit&lt;/strong&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Vermindert Schuldfähige werden als &lt;strong&gt;schuldfähig behandelt&lt;/strong&gt;, es ist aber ein &lt;strong&gt;Milderungsgrund &lt;/strong&gt;für die Strafbemessung.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann wird die Schuldfähigkeit ausgeschlossen?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;wegen&lt;strong&gt; mangelnder Reife&lt;/strong&gt; (&lt;a href="https://www.jusline.at/gesetz/jgg/paragraf/4" rel="noopener noreferrer" target="_blank"&gt;§ 4 JGG&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Unmündige (bis 14 Jahre)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Jugendliche (14 bis 18 Jahre) nur bei verzögerter Reife&lt;/li&gt;&lt;li&gt;wegen &lt;strong&gt;seelischer Störungen &lt;/strong&gt;(&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/11" rel="noopener noreferrer" target="_blank"&gt;§ 11 StGB&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Geisteskrankheit&lt;/li&gt;&lt;li class="ql-indent-1"&gt;geistige Behinderung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;tiefgreifende Bewusstseinsstörung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;gleichwertige seelische Störung&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Kann ein Schuldunfähiger rechtswidrig handeln?&lt;/p&gt;&lt;p&gt;Kann er bestraft werden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Er kann rechtswidrig handeln, aber&lt;strong&gt; nicht bestraft&lt;/strong&gt; werden.&lt;/li&gt;&lt;li&gt;Stattdessen kann eine vorbeugende Maßnahme in Betracht kommen.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Aus welchen zwei Fähigkeiten besteht die Schuldfähigkeit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Einsichts/Diskretionsfähigkeit&lt;/li&gt;&lt;li&gt;Steuerungs/Dispositionsfähigkeit&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die zeitliche Einschränkung der Schuldfähigkeit in Bezug auf die Tat?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Beide Teile der Schuldfähigkeit müssen zur Zeit der Tat vorhanden sein &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Schuldfähigkeit?&lt;/p&gt;&lt;p&gt;Wie wird sie noch genannt?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/11" rel="noopener noreferrer" target="_blank"&gt;§ 11 StGB &lt;/a&gt;Fähigkeit, das &lt;strong&gt;Unrecht &lt;/strong&gt;der Tat &lt;strong&gt;einzusehen, &lt;/strong&gt;nd &lt;strong&gt;nach &lt;/strong&gt;dieser &lt;strong&gt;Einsicht &lt;/strong&gt;zu &lt;strong&gt;handeln &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ist die &lt;strong&gt;irrtümliche &lt;/strong&gt;Annahme eine Strafausschließungsgrundes relevant für Schuld oder Strafe?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Weder für Schuld noch Strafe beachtlich&lt;/strong&gt;, auf die Vorstellung des Täters von einem Strafausschließungsgrund kommt es nicht an,&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Versuchsdelikte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Das Gesetz erklärt schon die &lt;strong&gt;Vornahme des Versuchs &lt;/strong&gt;zur vollendeten Tat.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Vorbereitungs&lt;strong&gt;delikte&lt;/strong&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Delikte, die bestimmte Vorbereitungshandlungen mit Strafe bedrohen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Vorbereitungs&lt;strong&gt;handlungen&lt;/strong&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Handlungen, welche die &lt;strong&gt;spätere&lt;/strong&gt; &lt;strong&gt;Ausführung &lt;/strong&gt;der Tat&lt;strong&gt; ermöglichen&lt;/strong&gt;, &lt;strong&gt;erleichtern&lt;/strong&gt; oder &lt;strong&gt;absichern &lt;/strong&gt;sollen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Kann für Entschließung und Vorbereitung eines vorsätzlichen Delikts gestraft werden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sind idR straflos&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die 4 Stadien des vorsätzlichen Delikts?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;Entschließung&lt;/li&gt;&lt;li&gt;Vorbereitung&lt;/li&gt;&lt;li&gt;Versuch&lt;/li&gt;&lt;li&gt;Vollendung&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die Irrige Annahme eines &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;rechtfertigenden &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Sachverhalts? &lt;/span&gt;&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;Was sind die Rechtsfolgen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Täter nimmt irrtümlich einen Sachverhalt an, der die Rechtswidrigkeit der Tat ausschließen würde&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/8" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(170, 160, 247);"&gt;§ 8 S1 StGB&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Folgen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(170, 160, 247);"&gt;Keine Bestrafung wegen vorsätzlicher Tat&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bestrafung wegen fahrlässiger Tat durch&lt;strong&gt; &lt;/strong&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;doppelt bedingte Fahrlässigkeit&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die doppelt bedingte Fahrlässigkeitshaftung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Bestrafung wegen fahrlässiger Tat, wenn es ein &lt;strong&gt;entsprechendes &lt;/strong&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Fahrlässigkeitsdelikt &lt;/strong&gt;gibt, und der &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Irrtum auf Fahrlässigkeit beruht&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die irrige Annahme eines &lt;strong&gt;entschuldigenden &lt;/strong&gt;Sachverhalts?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;Was sind die Rechtsfolgen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Täter nimmt &lt;strong&gt;irrtümlich &lt;/strong&gt;einen Sachverhalt an, der die &lt;strong&gt;rechtswidrige Tat entschuldigen &lt;/strong&gt;würde.&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/10" rel="noopener noreferrer" target="_blank" style="color: rgb(170, 160, 247); background-color: rgb(40, 45, 88);"&gt;§ 10 (2) StGB&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Folgen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="color: rgb(170, 160, 247); background-color: rgb(40, 45, 88);"&gt;Keine Bestrafung wegen vorsätzlicher Tat&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bestrafung wegen fahrlässiger Tat durch&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;doppelt bedingte Fahrlässigkeit&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die &lt;strong&gt;Rettungsabsicht &lt;/strong&gt;beim entschuldigenden Notstand?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der Notstand &lt;strong&gt;setzt&lt;/strong&gt; &lt;strong&gt;Rettungsabsicht &lt;/strong&gt;("um abzuwenden") &lt;strong&gt;voraus &lt;/strong&gt;(Es reicht aus über eine Notstandssituation zu wissen, man muss rettend handeln), sonst bleibt es bei Bestrafung für vorsätzliche Tat&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Kriterien muss die Notstands&lt;strong&gt;handlung&lt;/strong&gt; erfüllen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Notwendig &lt;/strong&gt;und&lt;strong&gt; geeignet &lt;/strong&gt;zur Abwendung des Nachteils.&lt;/p&gt;&lt;p&gt;Sie muss aber &lt;strong&gt;nicht&lt;/strong&gt; das einzige oder mildeste Mittel sein.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Notstands&lt;strong&gt;situation&lt;/strong&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Unmittelbar drohender Nachteil für Individualrechtsgüter des Notstandstäters oder eines Dritten&lt;/p&gt;&lt;p&gt;Siehe &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/10" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(170, 160, 247);"&gt;§ 10 (1) StGB&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Rechtsgrundlage für den entschuldigenden Notstand? &lt;/p&gt;&lt;p&gt;Auf welche Arten von Delikten ist er anwendbar?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/10" rel="noopener noreferrer" target="_blank" style="color: rgb(170, 160, 247); background-color: rgb(40, 45, 88);"&gt;§ 10 (1) StGB&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="color: rgb(170, 160, 247); background-color: rgb(40, 45, 88);"&gt;nur auf &lt;/span&gt;&lt;strong style="color: rgb(170, 160, 247); background-color: rgb(40, 45, 88);"&gt;vorsätzliche Begehungsdelikte&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie wirken Entschuldigungsgründe?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die T&lt;strong&gt;at bleibt rechtswidrig&lt;/strong&gt;, aber die &lt;strong&gt;Schuld entfällt&lt;/strong&gt; und es kann nicht mehr bestraft werden.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der &lt;strong&gt;maßgerechte Mensch&lt;/strong&gt;?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage für die Definition?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/10" rel="noopener noreferrer" target="_blank"&gt;§ 10 (1) StGB&lt;/a&gt; Ein Mensch der sich mit den rechtlich geschützten werten verbunden fühlt.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Maßstab für die Zumutbarkeit des rechtmäßigen Verhaltens?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der maßgerechte Mensch&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Worum geht es bei den Entschuldigungsgründen?&lt;/p&gt;&lt;p&gt;Was ist die Folge eines Entschuldigungsgrundes?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Um die &lt;strong&gt;Zumutbarkeit rechtmäßigen Verhaltens.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Ist es nicht mehr zumutbar, ist der Täter entschuldigt und kann &lt;strong&gt;nicht bestraft&lt;/strong&gt; werden.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Subsumtionsirrtum?&lt;/p&gt;&lt;p&gt;Ist er ein Fall von Verbotsirrtum?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Täter &lt;strong&gt;erkennt Unrecht&lt;/strong&gt;, subsumiert Tat aber&lt;strong&gt; nicht unter die maßgebliche Strafvorschrift&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Dies ist ein &lt;strong&gt;Irrtum über die Strafbarkeit&lt;/strong&gt;, und daher unbeachtlich&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Was ist das Verhältnis zwischen &lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;Verbotsirrtum &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;und &lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;Strafbarkeitsirrtum (&lt;/strong&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;fehlendes Bewusstsein der Strafbarkeit&lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;)&lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;?&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
@@ -37,156 +421,6 @@
     <t>&lt;p&gt;&lt;strong&gt;Bewusstsein der Strafbarkeit&lt;/strong&gt; ist &lt;strong&gt;keine Voraussetzung &lt;/strong&gt;für Schuld oder Strafe. Relevant ist nur Bewusstsein des Unrechts.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist das Verhältnis zwischen &lt;strong&gt;Verbotsirrtum &lt;/strong&gt;und &lt;strong&gt;Tatbildirrtum&lt;/strong&gt;?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Tatbildirrtum&lt;/strong&gt;: Der Täter erkennt nicht, dass er einen Sachverhalt verwirklicht, der einem gesetzlichen Tatbild entspricht &lt;/li&gt;&lt;li class="ql-indent-1"&gt;bezieht sich also auf die &lt;strong&gt;tatsächliche &lt;/strong&gt;Seite&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verbotsirrtum&lt;/strong&gt;: Täter kennt Sachverhalt, weis aber nicht über das Unrecht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;bezieht sich also auf die &lt;strong&gt;rechtliche &lt;/strong&gt;Seite&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie verhält sich der &lt;strong&gt;vorwerfbare Verbotsirrtum &lt;/strong&gt;zum &lt;strong&gt;potenziellen&lt;/strong&gt; &lt;strong&gt;Unrechtsbewusstsein&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Synonym&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Beide bringen zum Ausdruck, dass der Täter das &lt;strong&gt;Unrecht nicht&lt;/strong&gt; &lt;strong&gt;erkannt &lt;/strong&gt;hat, aber sich hätte &lt;strong&gt;erkundigen müssen&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Ist Verbotsirrtum in der Praxis im Regelfall vorwerfbar oder nicht?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Im Regelfall vorwerfbar → Schuld und Strafbarkeit bleiben bestehen.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die Rechtsfolgen des Verbotsirrtums?&lt;/p&gt;&lt;p&gt;Was ist die Voraussetzung für den Eintritt?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Schuld und damit Strafe werden ausgeschlossen (&lt;strong&gt;Schuldausschließungsgrund&lt;/strong&gt;)&lt;/li&gt;&lt;li&gt;Voraussetzung: Verbotsirrtum muss &lt;strong&gt;nic&lt;span class="ql-cursor"&gt;﻿&lt;/span&gt;ht vorwerfbar &lt;/strong&gt;sein.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie wird der Verbotsirrtum in der Praxis gehandhabt?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Geht meist ins Leere da bereits &lt;strong&gt;latentes &lt;/strong&gt;oder &lt;strong&gt;laienmäßiges Unrechtsbewusstsein &lt;/strong&gt;Verbotsirrtum ausschließt&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die zwei Arten des Verbotsirtums?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;direkter &lt;/strong&gt;Verbotsirrtum: Täter &lt;strong&gt;erkennt nicht&lt;/strong&gt;, dass seine Tat verboten/unrecht ist&lt;/li&gt;&lt;li&gt;&lt;strong&gt;indirekter &lt;/strong&gt;Verbotsirrtum: Täter &lt;strong&gt;irrt über&lt;/strong&gt; Existenz/Grenzen eines &lt;strong&gt;Rechtfertigungsgrundes &lt;/strong&gt;-&amp;gt; er weiß, dass die Tat verboten ist, denkt aber sie er darf sie ausnahmsweise begehen&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie heißt der Verbotsirrtum im StGB (&lt;strong&gt;Rechtsgrundlage&lt;/strong&gt;)?&lt;/p&gt;&lt;p&gt;Warum wird der Begriff Verbotsirrtum im Schrifttum bevorzugt?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Rechtsirrtum gem &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/9" rel="noopener noreferrer" target="_blank"&gt;§ 9 StGB&lt;/a&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der Verbotsirrtum?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Der Täter &lt;strong&gt;erkennt das Unrecht seiner Tat nicht&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;-&amp;gt; Umkehr des Unrechtsbewusstseins&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist das Verhältnis zwischen Unrechtsbewusstsein und Tatvorsatz?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Vorsatz&lt;/strong&gt;: bezieht sich auf &lt;strong&gt;tatsächliche Seite &lt;/strong&gt;der Tat&lt;/li&gt;&lt;li class="ql-indent-1"&gt;muss &lt;strong&gt;tatsächlich vorhanden &lt;/strong&gt;sein.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Unrechtsbewusstsein&lt;/strong&gt;: bezieht sich auf die rechtliche Seite (Bewertung der Tat als Unrecht)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;muss nur &lt;strong&gt;potenziell vorhanden &lt;/strong&gt;sein.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist potenzielles Unrechtsbewusstsein?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Vorwerfbarer Mangel &lt;/strong&gt;des Unrechtsbewusstseins&lt;/li&gt;&lt;li&gt;Der Täter &lt;strong&gt;erkennt &lt;/strong&gt;das &lt;strong&gt;Unrecht&lt;/strong&gt; der Tat &lt;strong&gt;nicht&lt;/strong&gt;, wäre aber &lt;strong&gt;verpflichtet &lt;/strong&gt;gewesen sich danach &lt;strong&gt;zu erkundigen&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist aktuelles Unrechtsbewusstsein?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Zur Zeit der tat &lt;strong&gt;wirklich vorhandenes &lt;/strong&gt;Unrechtsbewusstsein.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist das Unrechtsbewusstsein? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Das Bewusstsein, dass die Tat gegen die Rechtsordnung verstößt.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der Unterschied zwischen alic und § 287 (1) StGB&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Erfüllen &lt;strong&gt;ähnliche Funktionen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;alic&lt;/strong&gt;: Vorsatz/Fahrlässigkeit bezieht sich auf die konkrete rechtswidrige Tat&lt;/li&gt;&lt;li&gt;&lt;strong&gt;287 (1)&lt;/strong&gt;: bestraft, wer die im Rausch begangenen Tat &lt;strong&gt;weder gewollt noch vorausgesehen hat&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie funktioniert die Schuldprüfung bei &lt;strong&gt;alic&lt;/strong&gt;?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Die Schuldprüfung wird auf den &lt;strong&gt;Zeitpunkt&lt;/strong&gt; &lt;strong&gt;verlegt&lt;/strong&gt;, in dem sich der Täter &lt;strong&gt;in den Zustand der Schuldunfähigkeit versetzt hat&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(226, 148, 20);"&gt;fahrlässige &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;actio libera in causa?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Täter versetzt sich in einen die Schuldfähigkeit ausschließenden Rauschzustand, obwohl er &lt;strong&gt;voraussehen hätte müssen&lt;/strong&gt;, dass er in diesem Zustand ein &lt;strong&gt;bestimmtes Delikt begehen wird.&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die &lt;strong&gt;vorsätzliche &lt;/strong&gt;actio libera in causa?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Täter hat sich mit dem &lt;strong&gt;Vorsatz &lt;/strong&gt;in den Status der Schuldunfähigkeit versetzt, in diesem&lt;strong&gt; Zustand eine rechtswidrige Tat zu begehen.&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wofür steht &lt;strong&gt;alic&lt;/strong&gt;?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Actio libera in causa&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die &lt;strong&gt;partielle &lt;/strong&gt;Schuld&lt;strong&gt;unfähigkeit&lt;/strong&gt;?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Schuldunfähigkeit trifft nur &lt;strong&gt;Teile des Unrechts&lt;/strong&gt;, d.h. § 11 wird n&lt;strong&gt;ur für manche Delikte&lt;/strong&gt; angewandt.&lt;/li&gt;&lt;li&gt;z.B.: Schuldunfähig für krankheitsspezifische Straftaten, für alles andere aber voll Schuldfähig&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die &lt;strong&gt;verminderte &lt;/strong&gt;Schuld&lt;strong&gt;fähigkeit&lt;/strong&gt;?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Vermindert Schuldfähige werden als &lt;strong&gt;schuldfähig behandelt&lt;/strong&gt;, es ist aber ein &lt;strong&gt;Milderungsgrund &lt;/strong&gt;für die Strafbemessung.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wann wird die Schuldfähigkeit ausgeschlossen?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;wegen&lt;strong&gt; mangelnder Reife&lt;/strong&gt; (&lt;a href="https://www.jusline.at/gesetz/jgg/paragraf/4" rel="noopener noreferrer" target="_blank"&gt;§ 4 JGG&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Unmündige (bis 14 Jahre)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Jugendliche (14 bis 18 Jahre) nur bei verzögerter Reife&lt;/li&gt;&lt;li&gt;wegen &lt;strong&gt;seelischer Störungen &lt;/strong&gt;(&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/11" rel="noopener noreferrer" target="_blank"&gt;§ 11 StGB&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Geisteskrankheit&lt;/li&gt;&lt;li class="ql-indent-1"&gt;geistige Behinderung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;tiefgreifende Bewusstseinsstörung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;gleichwertige seelische Störung&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Kann ein Schuldunfähiger rechtswidrig handeln?&lt;/p&gt;&lt;p&gt;Kann er bestraft werden?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Er kann rechtswidrig handeln, aber&lt;strong&gt; nicht bestraft&lt;/strong&gt; werden.&lt;/li&gt;&lt;li&gt;Stattdessen kann eine vorbeugende Maßnahme in Betracht kommen.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Aus welchen zwei Fähigkeiten besteht die Schuldfähigkeit?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Einsichts/Diskretionsfähigkeit&lt;/li&gt;&lt;li&gt;Steuerungs/Dispositionsfähigkeit&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die zeitliche Einschränkung der Schuldfähigkeit in Bezug auf die Tat?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Beide Teile der Schuldfähigkeit müssen zur Zeit der Tat vorhanden sein &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Schuldfähigkeit?&lt;/p&gt;&lt;p&gt;Wie wird sie noch genannt?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/11" rel="noopener noreferrer" target="_blank"&gt;§ 11 StGB &lt;/a&gt;Fähigkeit, das &lt;strong&gt;Unrecht &lt;/strong&gt;der Tat &lt;strong&gt;einzusehen, &lt;/strong&gt;nd &lt;strong&gt;nach &lt;/strong&gt;dieser &lt;strong&gt;Einsicht &lt;/strong&gt;zu &lt;strong&gt;handeln &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der Subsumtionsirrtum?&lt;/p&gt;&lt;p&gt;Ist er ein Fall von Verbotsirrtum?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Täter &lt;strong&gt;erkennt Unrecht&lt;/strong&gt;, subsumiert Tat aber&lt;strong&gt; nicht unter die maßgebliche Strafvorschrift&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Dies ist ein &lt;strong&gt;Irrtum über die Strafbarkeit&lt;/strong&gt;, und daher unbeachtlich&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Poena naturalis = natürliche Strafe&lt;/p&gt;</t>
   </si>
   <si>
@@ -928,7 +1162,7 @@
     <t>&lt;p&gt;Welche Bestrafung ist trotz Tatbildirrtum möglich?&lt;/p&gt;&lt;p&gt;Was sind die Voraussetzungen?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;ul&gt;&lt;li&gt;Bestrafung wegen &lt;strong&gt;fahrlässiger &lt;/strong&gt;Tat.&lt;/li&gt;&lt;li&gt;Es gibt ein &lt;strong&gt;entsprechendes Fahrlässigkeitsdelikt&lt;/strong&gt;, und der &lt;strong&gt;Irrtum beruht auf Fahrlässigkeit&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;ul&gt;&lt;li&gt;Bestrafung wegen &lt;strong&gt;fahrlässiger &lt;/strong&gt;Tat.&lt;/li&gt;&lt;li&gt;Voraussetzung: &lt;strong&gt;doppelt bedingte &lt;/strong&gt;Fahrlässigkeit&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was ist der Irrtum über das Tatobjekt (Objektsirrtum)?&lt;/p&gt;&lt;p&gt;Welche Arten gibt es, und begründen sie Tatbildirrtum?&lt;/p&gt;</t>
@@ -1723,7 +1957,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B221"/>
+  <dimension ref="A1:B260"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -3318,183 +3552,495 @@
         <v>396</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>361</v>
+        <v>397</v>
       </c>
     </row>
     <row r="200" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="201" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="202" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="203" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="204" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="205" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="206" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="207" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="208" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="209" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="210" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="211" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="212" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="213" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="214" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="215" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="216" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="217" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="218" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="219" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="220" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="221" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A222" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A223" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A224" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A225" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A226" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A227" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A228" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="B228" s="2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A238" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="B238" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="B221" s="2" t="s">
-        <v>440</v>
+    </row>
+    <row r="239" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A240" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="B246" s="2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="B247" s="2" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A248" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="B248" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A249" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="B249" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A250" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A251" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="B251" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A252" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A253" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="B253" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A254" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="B254" s="2" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A255" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A256" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="B256" s="2" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A257" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A258" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="B258" s="2" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A259" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="B259" s="2" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A260" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="B260" s="2" t="s">
+        <v>518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add additional cards, sort into fitting (sub)course
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - VU Strafrecht I - 1. Klausur (JKU, Austria).xlsx
+++ b/flashcards/Memcode - VU Strafrecht I - 1. Klausur (JKU, Austria).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="453">
   <si>
     <t>Question</t>
   </si>
@@ -19,66 +19,60 @@
     <t>Answer</t>
   </si>
   <si>
+    <t>&lt;p&gt;Wie verhält sich das Wahndelikt zum Verbotsirrtum?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Das Wahndelikt ist ein &lt;strong&gt;Zuviel&lt;/strong&gt; an Unrechtsbewusstsein (Täter glaubt sein Handeln ist verboten)&lt;/li&gt;&lt;li&gt;Der Verbotsirrtum ist ein &lt;strong&gt;Zuwenig&lt;/strong&gt; an Unrechtsbewusstsein (Täter glaubt sein Handeln ist erlaubt)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein untauglicher Versuch?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Untauglich ist ein Versuch, der aus &lt;strong&gt;tatsächlichen&lt;/strong&gt; &lt;strong&gt;oder rechtlichen Gründen&lt;/strong&gt;, die im Subjekt, in der Handlung oder im Objekt schon von vornherein angelegt (= &lt;strong&gt;vorprogrammiert&lt;/strong&gt;) sind, &lt;strong&gt;nicht zur Vollendung der Tat führen kann.&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/15" rel="noopener noreferrer" target="_blank"&gt;§ 15 (3) StGB&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein Wahndelikt?&lt;/p&gt;&lt;p&gt;Ist es Strafbar?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;Wie wird es noch genannt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Täter nimmt &lt;strong&gt;irrtümlich &lt;/strong&gt;eine Verbotslage an, die ihn belasten würde &lt;/li&gt;&lt;li&gt;Gem &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/1" rel="noopener noreferrer" target="_blank"&gt;§ 1 StGB&lt;/a&gt; nicht Strafbar:  nullum crimen sine lege&lt;/li&gt;&lt;li&gt;Putativdelikt&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Ist zufälliges Scheitern ein untauglicher Versuch?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nein, weil &lt;strong&gt;Zufall nicht &lt;/strong&gt;im Subjekt, in der Handlung oder im Objekt &lt;strong&gt;vorprogrammiert &lt;/strong&gt;ist.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Theorie der &lt;strong&gt;gesetzmäßigen&lt;/strong&gt; &lt;strong&gt;Bedingung&lt;/strong&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Bezieht sich auf die naturgesetzlichen garantierten Folgen einer Handlung&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Fall über 200m ist tödlich&lt;/li&gt;&lt;li&gt;Schuss in den Kopf ist tödlich&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Reserve&lt;strong&gt;ursachen&lt;/strong&gt; und Reserve&lt;strong&gt;handlungen&lt;/strong&gt;?&lt;/p&gt;&lt;p&gt;Welche werden berücksichtigt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Mindermeinung zur Berücksichtigung der hypothetischen Kausalverläufe → nach hM aber unbeachtlich!&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Reserveursache&lt;/strong&gt;: Ist bereits im Gange, eine Umentscheidung ist nicht möglich&lt;/li&gt;&lt;li class="ql-indent-1"&gt;z.B.: Langsam wirkendes Gift bereits verabreicht&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Reservehandlungen&lt;/strong&gt;: Ist erst geplant, kann aber noch abgewendet werden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;z.B.: Messer gekauft, aber noch niemand erstochen&lt;/li&gt;&lt;li&gt;Berücksichtigt werden &lt;strong&gt;Reserveursachen&lt;/strong&gt;, Reservehandlungen nur, wenn sie rechtlich geboten sind&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind &lt;strong&gt;notwendige&lt;/strong&gt;, was sind &lt;strong&gt;hinreichende &lt;/strong&gt;Bedingungen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Notwendig:&lt;/strong&gt; Notwendig für Erfolg (bei Wegfall kein Erfolg)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Hinreichend: &lt;/strong&gt;Alleine verantwortlich für Erfolg (keine weiteren Bedingungen benötigt)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Handlungsqualität?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Eine Handlung hat Handlungsqualität, wenn sie eine vom &lt;strong&gt;Willen beherrschbare menschliche&lt;/strong&gt; &lt;strong&gt;Handlung &lt;/strong&gt;ist&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Was sind die Folgen vom Rücktritt vom untauglichen Versuch?&lt;/p&gt;&lt;p&gt;Welche zwei Arten gibt es? &lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;ul&gt;&lt;li&gt;Für &lt;strong&gt;absolut untauglichen &lt;/strong&gt;Versuch sowie &lt;strong&gt;untaugliches&lt;/strong&gt; &lt;strong&gt;Subjekt &lt;/strong&gt;unproblematisch, weil ohnehin &lt;strong&gt;straflos&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Rücktritt vom &lt;strong&gt;unbeendeten &lt;/strong&gt;untauglichen Versuch:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;freiwillige Aufgabe der Tatausführung genügt, &lt;strong&gt;einfacher &lt;/strong&gt;Rücktritt gem &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/16" rel="noopener noreferrer" target="_blank"&gt;§ 16 (1)&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Rücktritt vom &lt;strong&gt;beendeten &lt;/strong&gt;untauglichen Versuch:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;tätiger &lt;/strong&gt;Rücktritt &lt;strong&gt;unmöglich &lt;/strong&gt;(weil Vollendung gar nicht eintreten kann) → um Schlechterstellung gegenüber tauglichem Versuch zu verhindern: &lt;strong&gt;Putativrücktritt &lt;/strong&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/16" rel="noopener noreferrer" target="_blank"&gt;§ 16 (2) &lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Wie verhält sich das Wahndelikt zum Verbotsirrtum?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Das Wahndelikt ist ein &lt;strong&gt;Zuviel&lt;/strong&gt; an Unrechtsbewusstsein (Täter glaubt sein Handeln ist verboten)&lt;/li&gt;&lt;li&gt;Der Verbotsirrtum ist ein &lt;strong&gt;Zuwenig&lt;/strong&gt; an Unrechtsbewusstsein (Täter glaubt sein Handeln ist erlaubt)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist ein Wahndelikt?&lt;/p&gt;&lt;p&gt;Ist es Strafbar?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;Wie wird es noch genannt?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Täter nimmt &lt;strong&gt;irrtümlich &lt;/strong&gt;eine Verbotslage an, die ihn belasten würde &lt;/li&gt;&lt;li&gt;Gem &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/1" rel="noopener noreferrer" target="_blank"&gt;§ 1 StGB&lt;/a&gt; nicht Strafbar:  nullum crimen sine lege&lt;/li&gt;&lt;li&gt;Putativdelikt&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der absolut untaugliche Versuch?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsfolge?&lt;/p&gt;&lt;p&gt;Beispiele?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Vollendung &lt;/strong&gt;der Tat nach Tatplan gemäß Eindruckstheorie unmöglich&lt;/li&gt;&lt;li&gt;Folge: Straflosigkeit&lt;/li&gt;&lt;li&gt;z.B.: "tot-beten", Kind mit Kamillentee abtreiben wollen, ...&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Unterscheidet das StGB zwischen tauglichen und untauglichen Versuchen?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Nein, nur die wissenschaftliche Systematik unterscheidet&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Eindruckstheorie für den untauglichen Versuch?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Ein Versuch ist &lt;strong&gt;absolut untauglich&lt;/strong&gt;, wenn aus der Sicht eines &lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;verständigenden begleitenden Beobachters&lt;/strong&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt; die Verwirklichung des Tatplans&lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt; unter keinen Umständen&lt;/strong&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt; zur Vollendung der Tat führen kann.&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Sind untaugliche Versuche strafwürdig?&lt;/p&gt;&lt;p&gt;Worauf basiert diese Annahme? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Nach der &lt;strong&gt;Eindruckstheorie &lt;/strong&gt;ist jeder Versuch &lt;strong&gt;strafwürdig&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ausgenommen &lt;/strong&gt;ist nur der &lt;strong&gt;absolut&lt;/strong&gt; untaugliche Versuch&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die drei Ursachen für die Untauglichkeit des Versuchs?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Untauglichkeit des &lt;strong&gt;Subjekts (&lt;/strong&gt;straflos weil unmöglich&lt;strong&gt;)&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;z.B.: Eheschließung eines Verheirateten, der vom Tod seiner ersten Frau noch nichts weiß&lt;/li&gt;&lt;li&gt;Untauglichkeit des &lt;strong&gt;Objekts&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;z.B.: Griff des Diebes in die leere Jackentasche&lt;/li&gt;&lt;li class="ql-indent-1"&gt;z.B.: Schuss auf einen scheinbar Schlafenden, der aber schon tot ist.&lt;/li&gt;&lt;li&gt;Untauglichkeit der &lt;strong&gt;Handlung&lt;/strong&gt;: meist &lt;strong&gt;untaugliches Mittel&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;z.B.: Mordwaffe schießt nicht weit genug&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Ist zufälliges Scheitern ein untauglicher Versuch?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Nein, weil &lt;strong&gt;Zufall nicht &lt;/strong&gt;im Subjekt, in der Handlung oder im Objekt &lt;strong&gt;vorprogrammiert &lt;/strong&gt;ist.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist ein untauglicher Versuch?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Untauglich ist ein Versuch, der aus &lt;strong&gt;tatsächlichen&lt;/strong&gt; &lt;strong&gt;oder rechtlichen Gründen&lt;/strong&gt;, die im Subjekt, in der Handlung oder im Objekt schon von vornherein angelegt (= &lt;strong&gt;vorprogrammiert&lt;/strong&gt;) sind, &lt;strong&gt;nicht zur Vollendung der Tat führen kann.&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/15" rel="noopener noreferrer" target="_blank"&gt;§ 15 (3) StGB&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Poena naturalis = natürliche Strafe&lt;/p&gt;</t>
   </si>
   <si>
@@ -295,34 +289,10 @@
     <t>&lt;ul&gt;&lt;li&gt;Eine Handlung, die gegen die Rechtsordnung als Ganzes verstößt &lt;/li&gt;&lt;li&gt;Strafhandlung kein unrecht wenn Rechtsordnung sie billigt. Verstöße wie Notwehr, Einwilligung, Anhalterecht, ... &lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist der &lt;strong&gt;Erfolgsunwert&lt;/strong&gt;?&lt;/p&gt;&lt;p&gt;Welche weiteren &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Eigenschaften &lt;/span&gt;gehören zum Erfolgsunwert?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Besteht in der Verletzung/Gefährdung des Rechtsguts (Tatobjekts). &lt;/li&gt;&lt;li&gt;Grad und Schwere der Verletzung und Höhe des Schadens gehören zum Erfolgsunwert&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der &lt;strong&gt;Handlungsunwert&lt;/strong&gt;?&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Welche weiteren Eigenschaften gehören zum Handlungsunwert?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Wird durch die &lt;strong&gt;Art &lt;/strong&gt;und &lt;strong&gt;Weise &lt;/strong&gt;der &lt;strong&gt;Tatbegehung &lt;/strong&gt;bestimmt (Wie wurde die Tat begangen)&lt;/li&gt;&lt;li&gt;Dazu gehören auch personale Komponenten (Wer hat die Tat begangen)&lt;/li&gt;&lt;li&gt;Steigt mit Intensität bzw. Brutalität der angewendeten Gewalt, sowie Schwere der eingesetzten Drohung&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der &lt;strong style="color: rgb(226, 148, 20); background-color: rgba(0, 0, 0, 0);"&gt;Gesinnungsunwert&lt;/strong&gt;?&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88);"&gt;Welche weiteren Eigenschaften gehören zum &lt;/span&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(226, 148, 20);"&gt;Gesinnungsunwert&lt;/span&gt;&lt;span style="background-color: rgb(40, 45, 88);"&gt;?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Der in der Tat zum Ausdruck kommende &lt;strong&gt;Schuldgehalt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Insbesondere die &lt;strong&gt;Art&lt;/strong&gt; und &lt;strong&gt;Maß &lt;/strong&gt;der durch die Tat dokumentierten &lt;strong&gt;rechtsfeindlichen Einstellung &lt;/strong&gt;und &lt;strong&gt;kriminellen Energie &lt;/strong&gt;(vorsätzliche Tötung [Mord] vs fahrlässige Tötung)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wofür werden &lt;strong&gt;Erfolgs&lt;/strong&gt;-, &lt;strong&gt;Handlungs&lt;/strong&gt;- und &lt;strong&gt;Gesinnungsunwert &lt;/strong&gt;verwendet? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Für die Strafzumessung und Diversion&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was ist der Tatbestand?&lt;/p&gt;&lt;p&gt;Wie wird er noch genannt?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;ul&gt;&lt;li&gt;Die gesetzliche Beschreibung einer Handlung, die strafrechtliches Unrecht ist. &lt;/li&gt;&lt;li&gt;Unrechtstypus&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;ul&gt;&lt;li&gt;Die gesetzliche Beschreibung einer Handlung, die strafrechtliches Unrecht ist.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Unrechtstypus&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was sind Rechtfertigungsgründe?&lt;/p&gt;</t>
@@ -361,13 +331,7 @@
     <t>&lt;ul&gt;&lt;li&gt;Sie beseitigen nicht die &lt;strong&gt;Tatbestandsmäßigkeit&lt;/strong&gt;, sondern nur das &lt;strong&gt;Unrecht&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;Die Handlung wird von der Rechtsordnung gebilligt, es darf keine Strafe oder vorbeugende Maßnahme verhängt werden. &lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist die Vorrausetzung für die Wirkung eines Rechtfertigungsgrundes?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Sämtliche Merkmale des RFG müssen erfüllt sein.&lt;/li&gt;&lt;li&gt;Die Handlung bleibt unrecht/strafbar, wenn die Grenzen des RFg überschritten werden. &lt;/li&gt;&lt;li&gt;RFG wirkt nur &lt;strong&gt;ad personam&lt;/strong&gt; (persönlich), d.h. bei mehreren Beteiligten einer Tat ist nur derjenige gerechtfertigt, der in seiner Person alle Merkmale des RFG erfüllt.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist das Fallprüfungsschema?&lt;/p&gt;</t>
+    <t>&lt;p&gt;Was ist das allgemeine Fallprüfungsschema?&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;0. Handlungsbegriff (nur zu prüfen wenn indiziert!)&lt;/p&gt;&lt;p&gt;I. Tatbestand&lt;/p&gt;&lt;p&gt;II. Rechtswidrigkeit&lt;/p&gt;&lt;p&gt;III. Schuld&lt;/p&gt;</t>
@@ -385,22 +349,16 @@
     <t>&lt;ul&gt;&lt;li&gt;Für &lt;strong&gt;Schlafende &lt;/strong&gt;und &lt;strong&gt;Bewusstlose&lt;/strong&gt;, bei &lt;strong&gt;Körperreflexen &lt;/strong&gt;und bei &lt;strong&gt;vis absoluta&lt;/strong&gt; fehlt die Möglichkeit der willensmäßigen Beherrschung -&amp;gt; keine Bestrafung.&lt;/li&gt;&lt;li&gt;Es darf bei Schlafenden und Bewusstlosen nicht übersehen werden, dass sie möglicherweise &lt;strong&gt;bereits früher strafbar gehandelt&lt;/strong&gt; haben: z.B: Verkehrsunfall durch Sekundenschlaf -&amp;gt; erfüllt Handlungsbegriff, weil trotz Müdigkeit weitergefahren wurde.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Wie werden Körperreflexe für die Ausschlussfunktion abgegrenzt?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Fehlreaktionen eines Kraftfahrers &lt;/strong&gt;der von plötzlicher Gefahr überrascht wird, sind in den meisten Fällen vom Willen beherrschbar und erfüllen daher den strafrechtlichen Handlungsbegriff (auch Fehlreaktionen innerhalb der sog. Reaktionszeit)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Automatisierte Handlungen&lt;/strong&gt; sind eintrainierte Verhaltensweisen, bei denen der Wille nicht jedes mal aktiv eingeschalten wird, die Willensaktivierung kann aber jederzeit erfolgen. Deshalb erfüllen Sie den strafrechtlichen Handlungsbegriff. Z.B.: Schalten, Bremsen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Impulsive Handlungen&lt;/strong&gt; kommen zwar unter Umgehung der Tathemmungsmechanismen, nicht aber unter Ausschaltung des Willens zu stande, und erfüllen daher den &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;strafrechtlichen Handlungsbegriff. Z.B.: Affekt- und Kurzschlussreaktionen&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was ist vis absoluta?&lt;/p&gt;&lt;p&gt;Erfüllt sie den strafrechtlichen Handlungsbegriff?&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;willensausschließende&lt;/strong&gt;, in diesem Sinn &lt;strong&gt;unwiderstehliche &lt;/strong&gt;Gewalt. &lt;/li&gt;&lt;li&gt;Der Gezwungene ist&lt;strong&gt; physisch nicht in der Lage Widerstand zu leisten,&lt;/strong&gt; daher wird der &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;strafrechtliche Handlungsbegriff nicht erfüllt.&lt;/span&gt;&lt;/li&gt;&lt;li&gt;z.B: jemand wird vor ein Auto gestoßen, die Hand wird zum Testieren gewaltsam geführt.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist vis compulsiva?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;willensbeugende &lt;/strong&gt;Gewalt&lt;/li&gt;&lt;li&gt;Der Zwang ist nicht stark genug um den Willen des Gezwungenen auszuschließen, aber intensiv genug um den Willen zu beugen.&lt;/li&gt;&lt;li&gt;Z.B.: Jemand wird solange bedroht/verprügelt/eingesperrt, bis er die verlangte strafbare Handlung begeht.&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;p&gt;Was ist vis compulsiva?&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Erfüllt sie den strafrechtlichen Handlungsbegriff?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;willensbeugende &lt;/strong&gt;Gewalt&lt;/li&gt;&lt;li&gt;Der Zwang ist nicht stark genug um den Willen des Gezwungenen auszuschließen, aber intensiv genug um den Willen zu beugen.&lt;/li&gt;&lt;li&gt;Z.B.: Jemand wird solange bedroht/verprügelt/eingesperrt, bis er die verlangte strafbare Handlung begeht.&lt;/li&gt;&lt;li&gt;Gem &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/34" rel="noopener noreferrer" target="_blank"&gt;§ 34 (4) StGB&lt;/a&gt; ist vis compulsiva nur ein &lt;strong&gt;Milderungsgrund&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was sind Tun und Unterlassen?&lt;/p&gt;&lt;p&gt;Erfüllen Sie den strafrechtlichen Handlungsbegriff?&lt;/p&gt;</t>
@@ -451,12 +409,6 @@
     <t>&lt;ul&gt;&lt;li&gt;sind auslegungsbedürftig&lt;/li&gt;&lt;li&gt;Bedürfen der Ausfüllung anhand einer Werteordnung&lt;/li&gt;&lt;li&gt;manchmal enthält das Gesetz selbst Legaldefinitionen&lt;/li&gt;&lt;li&gt;z.B.: geschlechtliche Handlung, fremd, Bereicherungsvorsatz&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was sind &lt;strong&gt;geschriebene &lt;/strong&gt;und &lt;strong&gt;ungeschriebene &lt;/strong&gt;Tatbestandsmerkmale&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Geschriebene Tatbestandsmerkmale&lt;/strong&gt;: der Großteil der Merkmale ist &lt;strong&gt;ausdrücklich &lt;/strong&gt;im&lt;strong&gt; Gesetz festgelegt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Bei einer Reihe von Delikten kommen aber auch &lt;strong&gt;ungeschriebene Tatbestandsmerkmale&lt;/strong&gt; vor.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was ist teleologische Reduktion?&lt;/p&gt;</t>
   </si>
   <si>
@@ -652,7 +604,7 @@
     <t>&lt;p&gt;Was ist kumulative Kausalität?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Der Erfolg tritt durch das &lt;strong&gt;Zusammenwirken &lt;/strong&gt;mehrerer Handlungen ein. Damit ist jede dieser Handlungen kausal.&lt;/p&gt;</t>
+    <t>&lt;ul&gt;&lt;li&gt;Der Erfolg tritt durch das (gleichzeitige) &lt;strong&gt;Zusammenwirken &lt;/strong&gt;mehrerer Handlungen ein. Damit ist jede dieser Handlungen kausal.&lt;/li&gt;&lt;li&gt;Beispiel: Zwei Täter schießen exakt zur gleichen Zeit auf ein Opfer und beide Treffen es zeitgleich tödlich.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was ist überholende Kausalität?&lt;/p&gt;</t>
@@ -835,12 +787,6 @@
     <t>&lt;ul&gt;&lt;li&gt;Infolge von &lt;strong&gt;Abirren &lt;/strong&gt;(Fehlgehen) &lt;strong&gt;des&lt;/strong&gt; &lt;strong&gt;Angriffs &lt;/strong&gt;wird ein &lt;strong&gt;anderes als das anvisierte Objekt&lt;/strong&gt; (oder Person) getroffen.&lt;/li&gt;&lt;li&gt;sowohl bei gleichartigem als auch ungleichartigem Objekt ist &lt;strong&gt;Versuch hinsichtlich des gewollten Erfolgs&lt;/strong&gt; und unter Umständen &lt;strong&gt;fahrlässige Tat in Bezug auf tatsächlich eingetretenen Erfolg&lt;/strong&gt; anzunehmen → kein Entfall der Strafbarkeit aufgrund von Tatbildirrtum.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist dolus generalis?&lt;/p&gt;&lt;p&gt;Was ist die herrschende Ansicht dazu?&lt;/p&gt;&lt;p&gt;Welche Arten gibt es, und wie wirken Sie sich auf die Strafbarkeit aus?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Die ganze Tat umfassender "genereller Vorsatz"&lt;/li&gt;&lt;li&gt;Heute überholt, hA sieht einen &lt;strong&gt;Sonderfall des Irrtums über den Kausalverlauf &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Folgen (bei Änderung des Kausalverlaufs):&lt;/li&gt;&lt;li class="ql-indent-1"&gt;bei &lt;strong&gt;unwesentlicher &lt;/strong&gt;Änderung: Strafbarkeit für das &lt;strong&gt;vollendete Delikt.&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;z.B.: Täter wirft vermeintlich bereits getötetes Opfer in Fluss, Tod tritt erst durch Ertrinken ein. → Vollendeter Mord.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;bei &lt;strong&gt;wesentlicher &lt;/strong&gt;Änderung: Strafbarkeit wegen &lt;strong&gt;Versuchs&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;z.B.: Vermeintlich bereits getötetes Opfer ist im Kofferraum und stirbt erst durch Auffahrunfall → versuchter Mord.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was ist Irrtum über &lt;strong&gt;qualifizierende &lt;/strong&gt;Tatbestandsmerkmale?&lt;/p&gt;&lt;p&gt;Was ist die Ausnahme?&lt;/p&gt;</t>
   </si>
   <si>
@@ -928,7 +874,7 @@
     <t>&lt;p&gt;Schließen Zorn, Wut, Hass oder Vorsatz den Angreifer zu misshandeln/verletzen Notwehr aus?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Nein, wird dadurch nicht &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/3" rel="noopener noreferrer" target="_blank"&gt;§ 3 StGB&lt;/a&gt; ausgeschlossen.&lt;/p&gt;</t>
+    <t>&lt;p&gt;Nein, wird durch nicht &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/3" rel="noopener noreferrer" target="_blank"&gt;§ 3 StGB&lt;/a&gt; ausgeschlossen.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was ist Nothilfe?&lt;/p&gt;&lt;p&gt;Was ist die gesetzliche Grundlage?&lt;/p&gt;&lt;p&gt;Wie sind die &lt;strong&gt;Voraussetzungen des Angriffs&lt;/strong&gt; zu Beurteilen und bei wem muss das &lt;strong&gt;subjektive&lt;/strong&gt; &lt;strong&gt;Rechtfertigungselement &lt;/strong&gt;gegeben sein?&lt;/p&gt;</t>
@@ -1027,30 +973,6 @@
     <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/stpo/paragraf/80" rel="noopener noreferrer" target="_blank"&gt;§ 80 (2) StPO&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Jedermann ist zur &lt;strong&gt;angemessenen und zeitlich&lt;/strong&gt; &lt;strong&gt;begrenzten Anhaltung&lt;/strong&gt; eines Tatverdächtigen befugt (z.B.: Bei Ladendiebstählen)&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist die Anhaltesituation?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Verdacht der &lt;strong&gt;gegenwärtigen &lt;/strong&gt;oder &lt;strong&gt;unmittelbar&lt;/strong&gt; &lt;strong&gt;vorherigen Ausführung &lt;/strong&gt;einer strafbaren Handlung oder &lt;strong&gt;Fahndung &lt;/strong&gt;wegen einer solchen&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist eine strafbare Handlung im Sinne der Anhaltesituation?&lt;/p&gt;&lt;p&gt;Ist die Schuld(fähigkeit) relevant?&lt;/p&gt;&lt;p&gt;Wann entfällt das Anhalterecht?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Eine mit &lt;strong&gt;gerichtlicher Strafe bedrohte&lt;/strong&gt; &lt;strong&gt;Handlung&lt;/strong&gt;, auch Fahrlässigkeitsdelikte oder Bagatellstraftaten.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Schuld ist irrelevant&lt;/strong&gt;, es können auch Kinder, Jugendliche und Unzurechnungsfähige angehalten werden&lt;/li&gt;&lt;li&gt;Anhalterecht entfällt wenn die Strafdrohung entfällt (durch RFG gerechtfertigte Taten, strafbefreiender Rücktritt, ... )&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie wird die &lt;strong&gt;Anhaltedauer&lt;/strong&gt; begrenzt?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Wegall des Tatverdachts&lt;/strong&gt; (bei oder während der Festnahme) → Anhaltesituation entfällt und Anhaltung ist aufzuheben &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Unverzügliche Anzeige&lt;/strong&gt;: Anhaltung muss unverzüglich dem nächst erreichbaren Sicherheitsorgan angezeigt werden.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Wer die Anzeige verzögert oder unterlässt ist eventuell gem § 99 oder § 105 strafbar. &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist das &lt;strong&gt;subjektive Rechtfertigungselement &lt;/strong&gt;für die &lt;strong&gt;Anhaltedauer&lt;/strong&gt;?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Kenntnis der Anhaltesituation&lt;/strong&gt; genügt&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Ist die Anhaltung Unschuldiger gerechtfertigt?&lt;/p&gt;</t>
   </si>
   <si>
@@ -1069,30 +991,6 @@
     <t>&lt;ul&gt;&lt;li&gt;Privates Selbsthilferecht&lt;/li&gt;&lt;li&gt;Erlaubt, privatrechtliche Ansprüche in &lt;strong&gt;sehr engen Grenzen&lt;/strong&gt; im Wege der &lt;strong&gt;Selbsthilfe durchzusetzen&lt;/strong&gt; bzw. zu sichern.&lt;/li&gt;&lt;li&gt;Nur subsidiär (nachrangig)&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was sind die 2 Voraussetzungen für die Selbsthilfe&lt;strong&gt;situation&lt;/strong&gt;?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Bestehen eines &lt;strong&gt;privatrechtlichen Anspruchs&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Staatliche Hilfe kam &lt;strong&gt;zu spät&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;keine rechtzeitige Hilfe durch inländische Behörde/Organe (Gericht, Polizei, ...)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;es besteht also Gefahr, dass die Sicherung des Anspruchs vereitelt oder wesentlich erschwert wird.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was bedeutet die unbedingte Notwendigkeit bei der Selbsthilfehandlung?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Das schonendste Mittel&lt;/li&gt;&lt;li&gt;In Betracht kommen Identitätsfeststellung, einfache Drohungen, Festhalten, Ergreifen des Anspruchsgegenstands, ...&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Kann körperliche Gewalt bei der Selbsthilfe eingesetzt werden?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Vorsätzliche &lt;/strong&gt;Körperverletzung  (§ 83 (1) oder §§ 84f ) &lt;strong&gt;unzulässig &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Körperliche Misshandlungen (§ 83 (2) )bzw. &lt;strong&gt;fahrlässige&lt;/strong&gt; &lt;strong&gt;leichte &lt;/strong&gt;Körperverletzung gerechtfertigt.&lt;/li&gt;&lt;li&gt;Gegenwehr des Kontrahenten kann aber Notwehr oder Nothilfe rechtfertigen. &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist das subjektive Rechtfertigungselement in der Selbsthilfesituation?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Kenntnis der Selbsthilfesituation&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Deckt das allgemeine Selbsthilferecht auch Durchsetzung fremder privatrechtlicher Ansprüche (rechtfertigende Dritthilfe) ab?&lt;/p&gt;</t>
   </si>
   <si>
@@ -1102,42 +1000,12 @@
     <t>&lt;ul&gt;&lt;li&gt;Umfassender &lt;strong&gt;Rechtsschutzverzicht &lt;/strong&gt;durch &lt;strong&gt;bewusste Preisgabe&lt;/strong&gt; des Rechtsguts&lt;/li&gt;&lt;li&gt;Rechtsgrundlage: Rechtsordnung nimmt zwar Bezug darauf, aber definiert sie nicht → &lt;strong&gt;ungeschriebener Rechtfertigungsgrund&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Bezieht sich die Einwilligung auf die Handlung oder den Erfolg?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Auf den Erfolg&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Welche Anforderungen gibt es an die Einwilligung als &lt;strong&gt;Willenserklärung&lt;/strong&gt;?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;ausdrücklich oder konkludent&lt;/li&gt;&lt;li&gt;muss nach außen hin in Erscheinung treten&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was ist die Abgrenzung zwischen Einwilligung und Einverständnis? &lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;ul&gt;&lt;li&gt;Einwilligung wirkt &lt;strong&gt;rechtfertigend&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Einverständnis &lt;strong&gt;schließt&lt;/strong&gt; &lt;strong&gt;Tatbestand aus&lt;/strong&gt;, d.h. gibt es nur für Delikte deren Unwert aus &lt;strong&gt;Handeln ohne oder gegen den Willen des Rechtsträgers&lt;/strong&gt; kommt.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Benötigt die &lt;strong&gt;Dispositionsfähigkeit&lt;/strong&gt; die Geschäftsfähigkeit?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Nein, maßgeblich ist die &lt;strong&gt;natürliche Einsichts&lt;/strong&gt;- &lt;strong&gt;und Urteilsfähigkeit&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;z.B.: Einwilligung eines voll einsichtsfähigen Minderjährigen geht idR über die des gesetzlichen Vertreters.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie muss die &lt;strong&gt;Einwilligungshandlung &lt;/strong&gt;gestaltet sein?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Sie muss sich im Rahmen dessen halten, was der &lt;strong&gt;Rechtsgutsträger gewollt und erklärt hat&lt;/strong&gt;. Überschreitung → Handlungsexzess&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist das subjektive Rechtfertigungselement für die Einwilligung?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Der Täter muss &lt;strong&gt;aufgrund oder zumindest in Kenntnis der Einwilligung&lt;/strong&gt; des Betroffenen gehandelt haben.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was ist das Problem mit der Einwilligung zu Selbstgefährdung? &lt;/p&gt;</t>
   </si>
   <si>
@@ -1156,24 +1024,6 @@
     <t>&lt;ul&gt;&lt;li&gt;Wenn die &lt;strong&gt;Einwilligung nicht eingeholt werden kann&lt;/strong&gt; (Entscheidungsnotstand), der &lt;strong&gt;Rechtsgutsträger aber nach Lage der Dinge mit der Rechtsgutsbeeinträchtigung einverstanden gewesen wäre&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Ungeschriebener Rechtfertigungsgrund&lt;/li&gt;&lt;li&gt;z.B.: Bei Heilbehandlungen&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was sind die 2 Voraussetzungen für die &lt;strong&gt;mutmaßliche Einwilligungssituation&lt;/strong&gt;?&lt;/p&gt;&lt;p&gt;Was passiert bei Irrtum über die Einwilligungssituation? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Einwilligung&lt;/strong&gt; des Rechtsgutsträgers ist &lt;strong&gt;nicht erreichbar&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Hypothetischer Wille&lt;/strong&gt;: Hätte der Rechtsgutsträger in dieser Situation den willen erteilt? &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Anhand von objektiven Indizien aus der Sicht ex ante (vorher) zu ermitteln.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Irrtum &lt;/strong&gt;über hypothetischen Willen gem § 8 auf Fahrlässigkeit zu beurteilen.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die Grenzen der &lt;strong&gt;mutmaßlichen Einwilligungshandlung&lt;/strong&gt;?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Muss sich in den &lt;strong&gt;Grenzen &lt;/strong&gt;dessen halten, was der Rechtsgutsträger &lt;strong&gt;gewollt hätte&lt;/strong&gt;.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist das &lt;strong&gt;subjektive Rechtsfertigungselement &lt;/strong&gt;der &lt;strong&gt;mutmaßlichen Einwilligung&lt;/strong&gt;? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Wissen von &lt;strong&gt;Nichterreichbarkeit &lt;/strong&gt;des Rechtsgutsträgers&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Überzeugung&lt;/strong&gt;, dass dieser in der &lt;strong&gt;konkreten Situation&lt;/strong&gt; &lt;strong&gt;eingewilligt &lt;/strong&gt;hätte.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was ist das Schuldprinzip?&lt;/p&gt;&lt;p&gt;Welche Funktionen der Schuld können daraus abgeleitet werden? &lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
   </si>
   <si>
@@ -1192,12 +1042,6 @@
     <t>&lt;ul&gt;&lt;li&gt;Bezug auf &lt;strong&gt;rechtswidrige Tat&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Kann die rechtswidrige Tat dem Täter &lt;strong&gt;rechtlich zum Vorwurf &lt;/strong&gt;gemacht werden?&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist der &lt;strong&gt;objektive &lt;/strong&gt;Schuldmaßstab? &lt;/p&gt;&lt;p&gt;Wann hat der Täter dementsprechend schuldig gehandelt?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Maßstab der Schuld ist der &lt;strong&gt;maßgerechte Mensch in der Situation des Täters &lt;/strong&gt;(nicht die individuelle "Dafürkönnen" des Täters)&lt;/li&gt;&lt;li&gt;Der Täter hat schuldhaft gehandelt, wenn ein anderer in der Lage des Täters nach allgemeiner Erfahrung der Tatversuchung widerstanden hätte.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was ist die &lt;strong&gt;Vorsatz&lt;/strong&gt;schuld?&lt;/p&gt;</t>
   </si>
   <si>
@@ -1210,12 +1054,6 @@
     <t>&lt;p&gt;Mit dem Unwerturteil der Schuld wird dem Täter &lt;strong&gt;vorgeworfen&lt;/strong&gt;, dass er nicht jene ihm &lt;strong&gt;mögliche und zumutbare Sorgfalt eingehalten&lt;/strong&gt; hat, zu der er objektiv verpflichtet gewesen wäre.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was sind &lt;strong&gt;besondere Schuldmerkmale&lt;/strong&gt;?&lt;/p&gt;&lt;p&gt;Was welche sind dies in der Regel?&lt;/p&gt;&lt;p&gt;In welche 2 Arten wird unterschieden?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;schuldspezifische Umstände&lt;/strong&gt;, deren Vorliegen die &lt;strong&gt;Strafbarkeit herabsetzt&lt;/strong&gt; oder &lt;strong&gt;ausnahmsweise &lt;/strong&gt;erhöht.&lt;/li&gt;&lt;li&gt;idR situativ bedingte Gemütsverfassungen/zustände&lt;/li&gt;&lt;li&gt;Arten:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;objektivierte &lt;/strong&gt;Schuldmerkmale: schuldmindernde Gemütsverfassung wird &lt;strong&gt;ex lege unwiderleglich vermutet &lt;/strong&gt;(z.B.: "während der Geburt")   &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;subjektive &lt;/strong&gt;Schuldmerkmale: &lt;strong&gt;motivierende Wirkung &lt;/strong&gt;der besonderen Gemütsverfassung &lt;strong&gt;auf &lt;/strong&gt;die &lt;strong&gt;Willensbildung &lt;/strong&gt;muss &lt;strong&gt;in concreto nachgewiesen &lt;/strong&gt;werden &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was ist die Strafzumessungsschuld?&lt;/p&gt;&lt;p&gt;Was muss der Richter dabei berücksichtigen? &lt;/p&gt;</t>
   </si>
   <si>
@@ -1228,7 +1066,7 @@
     <t>&lt;p&gt;Durch normspezifische &lt;strong&gt;Auslegung&lt;/strong&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist die Schuldfähigkeit?&lt;/p&gt;&lt;p&gt;Wie wird sie noch genannt?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+    <t>&lt;p&gt;Was ist die Schuldfähigkeit?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/11" rel="noopener noreferrer" target="_blank"&gt;§ 11 StGB &lt;/a&gt;Fähigkeit, das &lt;strong&gt;Unrecht &lt;/strong&gt;der Tat &lt;strong&gt;einzusehen, &lt;/strong&gt;nd &lt;strong&gt;nach &lt;/strong&gt;dieser &lt;strong&gt;Einsicht &lt;/strong&gt;zu &lt;strong&gt;handeln &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
@@ -1258,18 +1096,6 @@
     <t>&lt;ul&gt;&lt;li&gt;wegen&lt;strong&gt; mangelnder Reife&lt;/strong&gt; (&lt;a href="https://www.jusline.at/gesetz/jgg/paragraf/4" rel="noopener noreferrer" target="_blank"&gt;§ 4 JGG&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Unmündige (bis 14 Jahre)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Jugendliche (14 bis 18 Jahre) nur bei verzögerter Reife&lt;/li&gt;&lt;li&gt;wegen &lt;strong&gt;seelischer Störungen &lt;/strong&gt;(&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/11" rel="noopener noreferrer" target="_blank"&gt;§ 11 StGB&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Geisteskrankheit&lt;/li&gt;&lt;li class="ql-indent-1"&gt;geistige Behinderung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;tiefgreifende Bewusstseinsstörung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;gleichwertige seelische Störung&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist die &lt;strong&gt;verminderte &lt;/strong&gt;Schuld&lt;strong&gt;fähigkeit&lt;/strong&gt;?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Vermindert Schuldfähige werden als &lt;strong&gt;schuldfähig behandelt&lt;/strong&gt;, es ist aber ein &lt;strong&gt;Milderungsgrund &lt;/strong&gt;für die Strafbemessung.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die &lt;strong&gt;partielle &lt;/strong&gt;Schuld&lt;strong&gt;unfähigkeit&lt;/strong&gt;?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Schuldunfähigkeit trifft nur &lt;strong&gt;Teile des Unrechts&lt;/strong&gt;, d.h. § 11 wird n&lt;strong&gt;ur für manche Delikte&lt;/strong&gt; angewandt.&lt;/li&gt;&lt;li&gt;z.B.: Schuldunfähig für krankheitsspezifische Straftaten, für alles andere aber voll Schuldfähig&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Wofür steht &lt;strong&gt;alic&lt;/strong&gt;?&lt;/p&gt;</t>
   </si>
   <si>
@@ -1294,7 +1120,7 @@
     <t>&lt;p&gt;Die Schuldprüfung wird auf den &lt;strong&gt;Zeitpunkt&lt;/strong&gt; &lt;strong&gt;verlegt&lt;/strong&gt;, in dem sich der Täter &lt;strong&gt;in den Zustand der Schuldunfähigkeit versetzt hat&lt;/strong&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist der Unterschied zwischen alic und § 287 (1) StGB&lt;/p&gt;</t>
+    <t>&lt;p&gt;Was ist der Unterschied zwischen alic und &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/287" rel="noopener noreferrer" target="_blank"&gt;§ 287 (1) StGB&lt;/a&gt; (Tat wärhend Berauschung)&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;ul&gt;&lt;li&gt;Erfüllen &lt;strong&gt;ähnliche Funktionen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;alic&lt;/strong&gt;: Vorsatz/Fahrlässigkeit bezieht sich auf die konkrete rechtswidrige Tat&lt;/li&gt;&lt;li&gt;&lt;strong&gt;287 (1)&lt;/strong&gt;: bestraft, wer die im Rausch begangenen Tat &lt;strong&gt;weder gewollt noch vorausgesehen hat&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
@@ -1306,24 +1132,6 @@
     <t>&lt;p&gt;Das Bewusstsein, dass die Tat gegen die Rechtsordnung verstößt.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist aktuelles Unrechtsbewusstsein?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Zur Zeit der tat &lt;strong&gt;wirklich vorhandenes &lt;/strong&gt;Unrechtsbewusstsein.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist potenzielles Unrechtsbewusstsein?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Vorwerfbarer Mangel &lt;/strong&gt;des Unrechtsbewusstseins&lt;/li&gt;&lt;li&gt;Der Täter &lt;strong&gt;erkennt &lt;/strong&gt;das &lt;strong&gt;Unrecht&lt;/strong&gt; der Tat &lt;strong&gt;nicht&lt;/strong&gt;, wäre aber &lt;strong&gt;verpflichtet &lt;/strong&gt;gewesen sich danach &lt;strong&gt;zu erkundigen&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Folge von Handlungen ohne aktuellem und potenziellem Unrechtsbewusstsein?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Schuld entfällt&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was ist das Verhältnis zwischen Unrechtsbewusstsein und Tatvorsatz?&lt;/p&gt;</t>
   </si>
   <si>
@@ -1348,12 +1156,6 @@
     <t>&lt;p&gt;Rechtsirrtum gem &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/9" rel="noopener noreferrer" target="_blank"&gt;§ 9 StGB&lt;/a&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was sind die zwei Arten des Verbotsirtums?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;direkter &lt;/strong&gt;Verbotsirrtum: Täter &lt;strong&gt;erkennt nicht&lt;/strong&gt;, dass seine Tat verboten/unrecht ist&lt;/li&gt;&lt;li&gt;&lt;strong&gt;indirekter &lt;/strong&gt;Verbotsirrtum: Täter &lt;strong&gt;irrt über&lt;/strong&gt; Existenz/Grenzen eines &lt;strong&gt;Rechtfertigungsgrundes &lt;/strong&gt;-&amp;gt; er weiß, dass die Tat verboten ist, denkt aber sie er darf sie ausnahmsweise begehen&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Wie wird der Verbotsirrtum in der Praxis gehandhabt?&lt;/p&gt;</t>
   </si>
   <si>
@@ -1426,24 +1228,6 @@
     <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/10" rel="noopener noreferrer" target="_blank" style="color: rgb(170, 160, 247); background-color: rgb(40, 45, 88);"&gt;§ 10 (1) StGB&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="color: rgb(170, 160, 247); background-color: rgb(40, 45, 88);"&gt;nur auf &lt;/span&gt;&lt;strong style="color: rgb(170, 160, 247); background-color: rgb(40, 45, 88);"&gt;vorsätzliche Begehungsdelikte&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist die Notstands&lt;strong&gt;situation&lt;/strong&gt;?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Unmittelbar drohender Nachteil für Individualrechtsgüter des Notstandstäters oder eines Dritten&lt;/p&gt;&lt;p&gt;Siehe &lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/10" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(170, 160, 247);"&gt;§ 10 (1) StGB&lt;/a&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Welche Kriterien muss die Notstands&lt;strong&gt;handlung&lt;/strong&gt; erfüllen?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Notwendig &lt;/strong&gt;und&lt;strong&gt; geeignet &lt;/strong&gt;zur Abwendung des Nachteils.&lt;/p&gt;&lt;p&gt;Sie muss aber &lt;strong&gt;nicht&lt;/strong&gt; das einzige oder mildeste Mittel sein.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die &lt;strong&gt;Rettungsabsicht &lt;/strong&gt;beim entschuldigenden Notstand?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Der Notstand &lt;strong&gt;setzt&lt;/strong&gt; &lt;strong&gt;Rettungsabsicht &lt;/strong&gt;("um abzuwenden") &lt;strong&gt;voraus &lt;/strong&gt;(Es reicht aus über eine Notstandssituation zu wissen, man muss rettend handeln), sonst bleibt es bei Bestrafung für vorsätzliche Tat&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was ist die irrige Annahme eines &lt;strong&gt;entschuldigenden &lt;/strong&gt;Sachverhalts?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;Was sind die Rechtsfolgen?&lt;/p&gt;</t>
   </si>
   <si>
@@ -1516,19 +1300,7 @@
     <t>&lt;ul&gt;&lt;li&gt;Vollständige Tat Versucht&lt;/li&gt;&lt;li&gt;Aber vor Vollendung "steckengeblieben"&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist das Fallprüfungsschema für den Tatbestand des Versuchs?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Nichterfüllung des gesetzlichen Tatbildes&lt;/strong&gt;: es dürfen nicht sämtliche objektiven Tatbestandmerkmale erfüllt sein&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Voller Tatentschluss&lt;/strong&gt;: Täter muss mit vollem Tatentschluss handeln (meist identisch mit Tatvorsatz)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ausführungshandlung bzw. ausführungsnahe Handlung&lt;/strong&gt;: sonst bloße Vorbereitungshandlung.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wann ist ein Versuch beendet, wann nicht?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Der Versuch ist beendet, wenn der &lt;strong&gt;Täter glaubt&lt;/strong&gt;, alles zur &lt;strong&gt;Vollendung&lt;/strong&gt; der Tat &lt;strong&gt;Erforderliche&lt;/strong&gt; &lt;strong&gt;getan&lt;/strong&gt; zu haben. &lt;/li&gt;&lt;li&gt;Glaubt er dagegen, noch &lt;strong&gt;weiterhandeln &lt;/strong&gt;zu müssen, ist der Versuch &lt;strong&gt;unbeendet&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Stellt das Beenden eines Versuchs einen Rücktritt nach § 16 dar?&lt;/p&gt;</t>
+    <t>&lt;p&gt;Stellt das Beenden eines Versuchs einen Rücktritt nach&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/16" rel="noopener noreferrer" target="_blank"&gt; § 16 &lt;/a&gt;dar?&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Nein, dafür müsste die &lt;strong&gt;Gefahr neutralisiert &lt;/strong&gt;werden ( gefahrneutralisierendes Handeln )&lt;/p&gt;</t>
@@ -1546,12 +1318,6 @@
     <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;einfacher &lt;/strong&gt;Rücktritt: vom &lt;strong&gt;unbeendeten &lt;/strong&gt;Versuch&lt;/li&gt;&lt;li&gt;&lt;strong&gt;tätiger &lt;/strong&gt;Rücktritt: vom &lt;strong&gt;beendeten &lt;/strong&gt;Versuch&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was sind die 2 Voraussetzungen für den Rücktritt vom &lt;strong&gt;unbeendeten &lt;/strong&gt;Versuch?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Endgültige &lt;/strong&gt;Aufgabe der Tatausführung: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Abbruch durch bloßes &lt;strong&gt;Nichtweiterhandeln &lt;/strong&gt;genügt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;endgültig: Täter &lt;strong&gt;verzichtet&lt;/strong&gt; auf &lt;strong&gt;weitere Ausführung&lt;/strong&gt;, bloße Unterbrechung reicht nicht&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Freiwilligkeit&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Frank&lt;/strong&gt;'sche und&lt;strong&gt; Roxin&lt;/strong&gt;'sche Formel (oft deckungsgleich, aber gut beide zur Gegenkontrolle zu verwenden) &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was ist die Frank'sche Formel für die Freiwilligkeit?&lt;/p&gt;</t>
   </si>
   <si>
@@ -1564,36 +1330,12 @@
     <t>&lt;ul&gt;&lt;li&gt;Der Rücktritt ist &lt;strong&gt;unfreiwillig&lt;/strong&gt;, wenn die Tat zwar objektiv noch ausführbar ist (oder der Täter sie für ausführbar hält), es aber &lt;strong&gt;iSd Verbrechervernunft unklug &lt;/strong&gt;wäre (angesichts der veränderten Umstände)&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Erfolg tritt trotz freiwilligem Rücktritt ein &lt;/p&gt;&lt;ul&gt;&lt;li&gt;Welche Folgen kann es geben?&lt;/li&gt;&lt;li&gt;Wie ist dieser Fall zu beurteilen?&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Straflos wegen Rücktritt oder Strafbar wegen vollendetem Delikt&lt;/li&gt;&lt;li&gt;Maßgeblich ist, ob der &lt;strong&gt;Eintritt des Erfolgs&lt;/strong&gt; nach Adäquanz- und Risikozusammmehang noch &lt;strong&gt;objektiv zugeordnet &lt;/strong&gt;werden kann&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was sind die 3 Voraussetzungen für den Rücktritt vom &lt;/span&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;beendeten &lt;/span&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Versuch?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Abwendung&lt;/strong&gt; des Erfolgs:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Strenge Anforderung: Erfolg muss &lt;strong&gt;tatsächlich &lt;/strong&gt;abgewendet werden.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Freiwilligkeit&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;Frank&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;'sche und&lt;/span&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt; &lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;Roxin&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;'sche Formel &lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;eigenes Zutun &lt;/strong&gt;des Täters:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;aktives&lt;/strong&gt; Gegensteuern durch gefahrneutralisierendes Handeln&lt;/li&gt;&lt;li class="ql-indent-1"&gt;passiv oder versehen &lt;strong&gt;reicht nicht&lt;/strong&gt;!&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist ein fehlgeschlagener Versuch?&lt;/p&gt;&lt;p&gt;Was sind die Rechtsfolgen?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Versuch ist fehlgeschlagen, wenn der Täter &lt;strong&gt;erkennt oder&lt;/strong&gt; &lt;strong&gt;glaubt&lt;/strong&gt;, dass sein er &lt;strong&gt;Ziel nicht mehr erreichen&lt;/strong&gt; kann (oder einen neuen Versuch bentigt)&lt;/li&gt;&lt;li&gt;Folgen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;kein Rücktritt oder Putativrücktritt möglich&lt;/li&gt;&lt;li class="ql-indent-1"&gt;also VOR Rücktritt zu prüfen.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was ist der Putativrücktritt?&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/16" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(115, 133, 197);"&gt;§ 16 (2) StGB&lt;/a&gt;: Erfolg bleibt &lt;strong&gt;ohne Zutun des Täters aus&lt;/strong&gt;, er ist sich dessen aber &lt;strong&gt;nicht bewusst &lt;/strong&gt;und nimmt &lt;strong&gt;ernstlich bemüht &lt;/strong&gt;einen &lt;strong&gt;Rücktritt &lt;/strong&gt;vor.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist ein qualifizierter Versuch? &lt;/p&gt;&lt;p&gt;Was ist die Folge hinsichtlich Rücktritt?&lt;/p&gt;&lt;p&gt;Beispiele?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Ein Versuch, in dem ein &lt;strong&gt;vollendetes Delikt enthalten &lt;/strong&gt;ist&lt;/li&gt;&lt;li&gt;Das im Versuch &lt;strong&gt;enthaltene Delikt &lt;/strong&gt;bleibt vom Rücktritt unberührt und daher &lt;strong&gt;strafbar&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;z.B.: Rücktritt von versuchtem Mord: Bestrafung wegen Körperverletzung&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was sind Strafaufhebungsgründe?&lt;/p&gt;&lt;p&gt;Was sind die 2 wichtigsten und deren Rechtsgrundlage?&lt;/p&gt;</t>
   </si>
   <si>
@@ -1621,7 +1363,7 @@
     <t>&lt;p&gt;Was sind Strafausschließungsgründe?&lt;/p&gt;&lt;p&gt;Was ist die wichtigste Rechtsgrundlage im Gerichtsalltag? &lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;ul&gt;&lt;li&gt;Umstände, die idR schon &lt;strong&gt;bei &lt;/strong&gt;der &lt;strong&gt;Begehung &lt;/strong&gt;der Straftat &lt;strong&gt;vorliegen &lt;/strong&gt;und einer &lt;strong&gt;Bestrafung &lt;/strong&gt;des Täters &lt;strong&gt;entgegenstehen&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;§ 88 (2) StGB&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;ul&gt;&lt;li&gt;Umstände, die idR schon &lt;strong&gt;bei &lt;/strong&gt;der &lt;strong&gt;Begehung &lt;/strong&gt;der Straftat &lt;strong&gt;vorliegen &lt;/strong&gt;und einer &lt;strong&gt;Bestrafung &lt;/strong&gt;des Täters &lt;strong&gt;entgegenstehen&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/stgb/paragraf/88" rel="noopener noreferrer" target="_blank"&gt;§ 88 (2) StGB&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Ist die &lt;strong&gt;irrtümliche &lt;/strong&gt;Annahme eine Strafausschließungsgrundes relevant für Schuld oder Strafe?&lt;/p&gt;</t>
@@ -2017,7 +1759,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B270"/>
+  <dimension ref="A1:B227"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -3332,143 +3074,143 @@
         <v>326</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
     </row>
     <row r="165" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B165" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="166" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B166" s="2" t="s">
         <v>330</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="167" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B167" s="2" t="s">
         <v>332</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="168" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B168" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="169" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B169" s="2" t="s">
         <v>336</v>
-      </c>
-      <c r="B169" s="2" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="170" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B170" s="2" t="s">
         <v>338</v>
-      </c>
-      <c r="B170" s="2" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="171" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B171" s="2" t="s">
         <v>340</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="172" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B172" s="2" t="s">
         <v>342</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="173" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B173" s="2" t="s">
         <v>344</v>
-      </c>
-      <c r="B173" s="2" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="174" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B174" s="2" t="s">
         <v>346</v>
-      </c>
-      <c r="B174" s="2" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="175" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B175" s="2" t="s">
         <v>348</v>
-      </c>
-      <c r="B175" s="2" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="176" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B176" s="2" t="s">
         <v>350</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="177" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B177" s="2" t="s">
         <v>352</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="178" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B178" s="2" t="s">
         <v>354</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="179" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B179" s="2" t="s">
         <v>356</v>
-      </c>
-      <c r="B179" s="2" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="180" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B180" s="2" t="s">
         <v>358</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="181" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B181" s="2" t="s">
         <v>360</v>
-      </c>
-      <c r="B181" s="2" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="182" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3837,350 +3579,6 @@
       </c>
       <c r="B227" s="2" t="s">
         <v>452</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A228" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="B228" s="2" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A229" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="B229" s="2" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="B230" s="2" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="231" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="B231" s="2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="B232" s="2" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A233" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="B233" s="2" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="234" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="B234" s="2" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="B235" s="2" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="B236" s="2" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="237" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A237" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="B237" s="2" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="B238" s="2" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="B239" s="2" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A240" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="B240" s="2" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="B241" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="242" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A242" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="B242" s="2" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A243" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="B243" s="2" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A244" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="B244" s="2" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="245" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A245" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="B245" s="2" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A246" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="B246" s="2" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A247" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="B247" s="2" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A248" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="B248" s="2" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A249" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="B249" s="2" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A250" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="B250" s="2" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A251" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="B251" s="2" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A252" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="B252" s="2" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A253" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="B253" s="2" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A254" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="B254" s="2" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A255" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="B255" s="2" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A256" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="B256" s="2" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="257" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A257" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="B257" s="2" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A258" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="B258" s="2" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A259" s="2" t="s">
-        <v>515</v>
-      </c>
-      <c r="B259" s="2" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A260" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="B260" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A261" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="B261" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A262" s="2" t="s">
-        <v>521</v>
-      </c>
-      <c r="B262" s="2" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A263" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="B263" s="2" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A264" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="B264" s="2" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A265" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="B265" s="2" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A266" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="B266" s="2" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A267" s="2" t="s">
-        <v>531</v>
-      </c>
-      <c r="B267" s="2" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A268" s="2" t="s">
-        <v>533</v>
-      </c>
-      <c r="B268" s="2" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A269" s="2" t="s">
-        <v>535</v>
-      </c>
-      <c r="B269" s="2" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A270" s="2" t="s">
-        <v>537</v>
-      </c>
-      <c r="B270" s="2" t="s">
-        <v>538</v>
       </c>
     </row>
   </sheetData>

</xml_diff>